<commit_message>
AFU, Indicatore 168 sostituito 9999999 con null
</commit_message>
<xml_diff>
--- a/earlywarning-pom/Document/SpecificheIndicatori/20161019 Indicatori EWS - Banche Italiane_SME_RETAIL.xlsx
+++ b/earlywarning-pom/Document/SpecificheIndicatori/20161019 Indicatori EWS - Banche Italiane_SME_RETAIL.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fernando.monaco\Desktop\ISP\SorgentiGIT\client-intesa\earlywarning-pom\Document\SpecificheIndicatori\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ilaria.cutano\Desktop\ISP\git\client-intesa\client-intesa\earlywarning-pom\Document\SpecificheIndicatori\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="468" windowWidth="31992" windowHeight="16272" tabRatio="918" firstSheet="2" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="468" windowWidth="31992" windowHeight="16272" tabRatio="918" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Legenda" sheetId="20" r:id="rId1"/>
@@ -3900,9 +3900,6 @@
     <t>Carta Commerciale</t>
   </si>
   <si>
-    <t>IND_164 &lt; 0.20 AND IND_165 &gt; 30</t>
-  </si>
-  <si>
     <t>IND_164 &gt;= 0.20 AND IND_165 &gt; 30</t>
   </si>
   <si>
@@ -3915,9 +3912,6 @@
     <t>Finanziamenti esteri - Finimport</t>
   </si>
   <si>
-    <t>IND_166 &lt; 0.20 AND IND_167 &gt; 30</t>
-  </si>
-  <si>
     <t>IND_166 &gt;= 0.20 AND IND_167 &gt; 30</t>
   </si>
   <si>
@@ -3925,9 +3919,6 @@
   </si>
   <si>
     <t>IND_167 = 0</t>
-  </si>
-  <si>
-    <t>IND_162 &lt; 0.20 AND IND_163 &gt; 60</t>
   </si>
   <si>
     <t>IND_162 &gt;= 0.20 AND IND_163 &gt; 60</t>
@@ -4386,6 +4377,15 @@
   </si>
   <si>
     <t>BR37</t>
+  </si>
+  <si>
+    <t>0,05 &lt;= IND_164 &lt; 0.20 AND IND_165 &gt; 30</t>
+  </si>
+  <si>
+    <t>0,05 &lt;= IND_166 &lt; 0.20 AND IND_167 &gt; 30</t>
+  </si>
+  <si>
+    <t>0,05 &lt;= IND_162 &lt; 0.20 AND IND_163 &gt; 60</t>
   </si>
 </sst>
 </file>
@@ -5484,7 +5484,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="464">
+  <cellXfs count="465">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -6673,72 +6673,6 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="8" borderId="9" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="8" borderId="10" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="8" borderId="23" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="8" borderId="24" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="8" borderId="0" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="49" fillId="4" borderId="2" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="9" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="10" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="23" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="24" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="0" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="13" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="13" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="13" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -6767,25 +6701,124 @@
     <xf numFmtId="0" fontId="15" fillId="31" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="8" borderId="9" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="8" borderId="10" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="8" borderId="23" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="8" borderId="24" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="8" borderId="0" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="4" borderId="2" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="9" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="10" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="23" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="24" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="0" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="13" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="13" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="13" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="Bad 2" xfId="2"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="7" builtinId="8"/>
     <cellStyle name="Normal 2" xfId="1"/>
     <cellStyle name="Normal 3" xfId="3"/>
     <cellStyle name="Normal 4" xfId="4"/>
     <cellStyle name="Normal 4 2" xfId="6"/>
     <cellStyle name="Normal 5" xfId="5"/>
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="101">
+  <dxfs count="91">
     <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
       <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC000"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF00B0F0"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF0070C0"/>
+          <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -7621,6 +7654,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C6500"/>
       </font>
       <fill>
@@ -7636,126 +7679,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF92D050"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC000"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF00B0F0"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF0070C0"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF92D050"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC000"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF00B0F0"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF0070C0"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF92D050"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC000"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF00B0F0"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF0070C0"/>
-          <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -8047,8 +7970,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:S30"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -8070,14 +7993,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="E1" s="430" t="s">
+      <c r="E1" s="442" t="s">
         <v>432</v>
       </c>
-      <c r="F1" s="430"/>
-      <c r="H1" s="431" t="s">
+      <c r="F1" s="442"/>
+      <c r="H1" s="443" t="s">
         <v>259</v>
       </c>
-      <c r="I1" s="432"/>
+      <c r="I1" s="444"/>
       <c r="J1" t="s">
         <v>254</v>
       </c>
@@ -8850,7 +8773,7 @@
       </c>
       <c r="L23" s="193"/>
       <c r="N23" s="136" t="s">
-        <v>966</v>
+        <v>963</v>
       </c>
       <c r="O23" s="136"/>
       <c r="P23" s="136" t="s">
@@ -8936,11 +8859,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="F1" s="449" t="s">
+      <c r="F1" s="461" t="s">
         <v>178</v>
       </c>
-      <c r="G1" s="449"/>
-      <c r="H1" s="449"/>
+      <c r="G1" s="461"/>
+      <c r="H1" s="461"/>
     </row>
     <row r="2" spans="1:8" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="168" t="s">
@@ -8954,34 +8877,34 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="445" t="s">
+      <c r="A3" s="457" t="s">
         <v>162</v>
       </c>
-      <c r="B3" s="446"/>
+      <c r="B3" s="458"/>
       <c r="C3" s="170"/>
       <c r="D3" s="195" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="445"/>
-      <c r="B4" s="447"/>
+      <c r="A4" s="457"/>
+      <c r="B4" s="459"/>
       <c r="C4" s="171"/>
       <c r="D4" s="196" t="s">
         <v>255</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="445"/>
-      <c r="B5" s="447"/>
+      <c r="A5" s="457"/>
+      <c r="B5" s="459"/>
       <c r="C5" s="171"/>
       <c r="D5" s="197" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="445"/>
-      <c r="B6" s="448"/>
+      <c r="A6" s="457"/>
+      <c r="B6" s="460"/>
       <c r="C6" s="172"/>
       <c r="D6" s="198" t="s">
         <v>166</v>
@@ -9036,7 +8959,7 @@
       <c r="O2" s="193"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A3" s="450"/>
+      <c r="A3" s="462"/>
       <c r="B3" s="176" t="s">
         <v>172</v>
       </c>
@@ -9059,7 +8982,7 @@
       <c r="O3"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A4" s="450"/>
+      <c r="A4" s="462"/>
       <c r="B4" s="154" t="s">
         <v>173</v>
       </c>
@@ -9080,7 +9003,7 @@
       <c r="O4" s="193"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A5" s="450"/>
+      <c r="A5" s="462"/>
       <c r="B5" s="154" t="s">
         <v>174</v>
       </c>
@@ -9101,7 +9024,7 @@
       <c r="O5" s="193"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A6" s="450"/>
+      <c r="A6" s="462"/>
       <c r="B6" s="154" t="s">
         <v>175</v>
       </c>
@@ -9122,7 +9045,7 @@
       <c r="O6" s="193"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A7" s="450"/>
+      <c r="A7" s="462"/>
       <c r="B7" s="154" t="s">
         <v>176</v>
       </c>
@@ -9172,7 +9095,7 @@
       <c r="O11"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A12" s="451"/>
+      <c r="A12" s="463"/>
       <c r="B12" s="176" t="s">
         <v>172</v>
       </c>
@@ -9195,7 +9118,7 @@
       <c r="O12"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A13" s="451"/>
+      <c r="A13" s="463"/>
       <c r="B13" s="154" t="s">
         <v>173</v>
       </c>
@@ -9216,7 +9139,7 @@
       <c r="O13"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A14" s="451"/>
+      <c r="A14" s="463"/>
       <c r="B14" s="154" t="s">
         <v>174</v>
       </c>
@@ -9237,7 +9160,7 @@
       <c r="O14"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A15" s="451"/>
+      <c r="A15" s="463"/>
       <c r="B15" s="154" t="s">
         <v>175</v>
       </c>
@@ -9258,7 +9181,7 @@
       <c r="O15"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A16" s="451"/>
+      <c r="A16" s="463"/>
       <c r="B16" s="154" t="s">
         <v>176</v>
       </c>
@@ -9654,30 +9577,30 @@
       <c r="V1" s="25"/>
       <c r="W1" s="25"/>
       <c r="X1" s="25"/>
-      <c r="Y1" s="433" t="s">
+      <c r="Y1" s="445" t="s">
         <v>12</v>
       </c>
-      <c r="Z1" s="434"/>
-      <c r="AA1" s="434"/>
-      <c r="AB1" s="435"/>
-      <c r="AC1" s="433" t="s">
+      <c r="Z1" s="446"/>
+      <c r="AA1" s="446"/>
+      <c r="AB1" s="447"/>
+      <c r="AC1" s="445" t="s">
         <v>13</v>
       </c>
-      <c r="AD1" s="434"/>
-      <c r="AE1" s="434"/>
-      <c r="AF1" s="435"/>
-      <c r="AG1" s="436" t="s">
+      <c r="AD1" s="446"/>
+      <c r="AE1" s="446"/>
+      <c r="AF1" s="447"/>
+      <c r="AG1" s="448" t="s">
         <v>14</v>
       </c>
-      <c r="AH1" s="437"/>
-      <c r="AI1" s="437"/>
-      <c r="AJ1" s="437"/>
-      <c r="AK1" s="436" t="s">
+      <c r="AH1" s="449"/>
+      <c r="AI1" s="449"/>
+      <c r="AJ1" s="449"/>
+      <c r="AK1" s="448" t="s">
         <v>68</v>
       </c>
-      <c r="AL1" s="437"/>
-      <c r="AM1" s="437"/>
-      <c r="AN1" s="437"/>
+      <c r="AL1" s="449"/>
+      <c r="AM1" s="449"/>
+      <c r="AN1" s="449"/>
     </row>
     <row r="2" spans="1:40" s="278" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A2" s="44" t="s">
@@ -12190,7 +12113,7 @@
       <c r="AM30" s="20"/>
       <c r="AN30" s="20"/>
     </row>
-    <row r="31" spans="1:40" ht="82.8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:40" ht="69" x14ac:dyDescent="0.3">
       <c r="A31" s="365" t="s">
         <v>72</v>
       </c>
@@ -12273,7 +12196,7 @@
       <c r="AM31" s="20"/>
       <c r="AN31" s="20"/>
     </row>
-    <row r="32" spans="1:40" s="289" customFormat="1" ht="165.6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:40" s="289" customFormat="1" ht="151.80000000000001" x14ac:dyDescent="0.3">
       <c r="A32" s="411" t="s">
         <v>72</v>
       </c>
@@ -12364,55 +12287,55 @@
     <mergeCell ref="AK1:AN1"/>
   </mergeCells>
   <conditionalFormatting sqref="T1:T2 T33:T1048576">
-    <cfRule type="cellIs" dxfId="85" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="90" priority="30" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="84" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="89" priority="32" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q33:S1048576 Q1:S2 Q4:R4 R5:R7 Q22:R22 R21 Q24:R27 R23 R28 Q29:R31 Q8:R20">
-    <cfRule type="cellIs" dxfId="83" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="88" priority="31" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q3:R3">
-    <cfRule type="cellIs" dxfId="82" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="87" priority="12" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R32">
-    <cfRule type="cellIs" dxfId="81" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="86" priority="10" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q5:Q7">
-    <cfRule type="cellIs" dxfId="80" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="85" priority="9" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q21">
-    <cfRule type="cellIs" dxfId="79" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="84" priority="7" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q28">
-    <cfRule type="cellIs" dxfId="78" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="83" priority="5" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q32">
-    <cfRule type="cellIs" dxfId="77" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="82" priority="3" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q23">
-    <cfRule type="cellIs" dxfId="76" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="81" priority="2" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S3:T32">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="80" priority="1" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12426,10 +12349,10 @@
   <dimension ref="A1:AO33"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="P3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="AD24" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="S3" sqref="S3"/>
+      <selection pane="bottomRight" activeCell="AL30" sqref="AL30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -12477,21 +12400,21 @@
       <c r="P1" s="27"/>
       <c r="Y1" s="70"/>
       <c r="Z1" s="70"/>
-      <c r="AB1" s="438" t="s">
+      <c r="AB1" s="450" t="s">
         <v>12</v>
       </c>
-      <c r="AC1" s="438"/>
-      <c r="AD1" s="438"/>
-      <c r="AE1" s="438" t="s">
+      <c r="AC1" s="450"/>
+      <c r="AD1" s="450"/>
+      <c r="AE1" s="450" t="s">
         <v>13</v>
       </c>
-      <c r="AF1" s="438"/>
-      <c r="AG1" s="438"/>
-      <c r="AH1" s="438" t="s">
+      <c r="AF1" s="450"/>
+      <c r="AG1" s="450"/>
+      <c r="AH1" s="450" t="s">
         <v>14</v>
       </c>
-      <c r="AI1" s="438"/>
-      <c r="AJ1" s="438"/>
+      <c r="AI1" s="450"/>
+      <c r="AJ1" s="450"/>
       <c r="AK1" s="105" t="s">
         <v>136</v>
       </c>
@@ -14322,7 +14245,7 @@
         <v>527</v>
       </c>
       <c r="P20" s="77" t="s">
-        <v>1029</v>
+        <v>1026</v>
       </c>
       <c r="Q20" s="6">
         <v>2</v>
@@ -15823,180 +15746,180 @@
     <mergeCell ref="AH1:AJ1"/>
   </mergeCells>
   <conditionalFormatting sqref="V1:V2 V34:V1048576">
-    <cfRule type="cellIs" dxfId="75" priority="126" operator="equal">
+    <cfRule type="cellIs" dxfId="79" priority="126" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="74" priority="128" operator="equal">
+    <cfRule type="cellIs" dxfId="78" priority="128" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R34:U1048576 R1:U2 Q16:V16 Q13 Q5:V6 AA14:AB14 R3:X33">
-    <cfRule type="cellIs" dxfId="73" priority="127" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="127" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V13:V14">
-    <cfRule type="cellIs" dxfId="72" priority="60" operator="equal">
+    <cfRule type="cellIs" dxfId="76" priority="60" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O6:P6">
-    <cfRule type="cellIs" dxfId="71" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="75" priority="45" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q35:Q1048576 Q1:Q2">
-    <cfRule type="cellIs" dxfId="70" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="74" priority="41" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q34">
-    <cfRule type="cellIs" dxfId="69" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="40" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q12">
-    <cfRule type="cellIs" dxfId="68" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="72" priority="36" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q15">
-    <cfRule type="cellIs" dxfId="67" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="71" priority="34" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q7">
-    <cfRule type="cellIs" dxfId="66" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="70" priority="32" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R7:V7">
-    <cfRule type="cellIs" dxfId="65" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="69" priority="31" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R22:V23">
-    <cfRule type="cellIs" dxfId="64" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="68" priority="28" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q22:Q23">
-    <cfRule type="cellIs" dxfId="63" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="27" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R22:V23">
-    <cfRule type="cellIs" dxfId="62" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="66" priority="26" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q22:Q23">
-    <cfRule type="cellIs" dxfId="61" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="25" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R3:V33">
-    <cfRule type="cellIs" dxfId="60" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="24" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q3:Q33">
-    <cfRule type="cellIs" dxfId="59" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="23" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R4:V4">
-    <cfRule type="cellIs" dxfId="58" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="22" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q4">
-    <cfRule type="cellIs" dxfId="57" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="21" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R10:V11">
-    <cfRule type="cellIs" dxfId="56" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="20" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q10:Q11">
-    <cfRule type="cellIs" dxfId="55" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="19" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R8:U8">
-    <cfRule type="cellIs" dxfId="54" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="15" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V8">
-    <cfRule type="cellIs" dxfId="53" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="14" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V8">
-    <cfRule type="cellIs" dxfId="52" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="13" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R9:U9 S3:S33">
-    <cfRule type="cellIs" dxfId="51" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="12" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V9">
-    <cfRule type="cellIs" dxfId="50" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="11" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V9">
-    <cfRule type="cellIs" dxfId="49" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="10" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R18:U21">
-    <cfRule type="cellIs" dxfId="48" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="9" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V18:V21">
-    <cfRule type="cellIs" dxfId="47" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="8" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O21">
-    <cfRule type="cellIs" dxfId="46" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="7" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V18:V21">
-    <cfRule type="cellIs" dxfId="45" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="6" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R24:V33">
-    <cfRule type="cellIs" dxfId="44" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="5" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V24:V33">
-    <cfRule type="cellIs" dxfId="43" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="4" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R17:X17">
-    <cfRule type="cellIs" dxfId="42" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="3" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q17">
-    <cfRule type="cellIs" dxfId="41" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="2" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R17:V17">
-    <cfRule type="cellIs" dxfId="40" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="1" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16010,10 +15933,10 @@
   <dimension ref="A1:AN15"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="S7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="S3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="U15" sqref="U15"/>
+      <selection pane="bottomRight" activeCell="U5" sqref="U5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -16058,30 +15981,30 @@
       <c r="P1" s="326"/>
       <c r="W1" s="330"/>
       <c r="X1" s="330"/>
-      <c r="Y1" s="439" t="s">
+      <c r="Y1" s="451" t="s">
         <v>12</v>
       </c>
-      <c r="Z1" s="440"/>
-      <c r="AA1" s="440"/>
-      <c r="AB1" s="441"/>
-      <c r="AC1" s="439" t="s">
+      <c r="Z1" s="452"/>
+      <c r="AA1" s="452"/>
+      <c r="AB1" s="453"/>
+      <c r="AC1" s="451" t="s">
         <v>13</v>
       </c>
-      <c r="AD1" s="440"/>
-      <c r="AE1" s="440"/>
-      <c r="AF1" s="441"/>
-      <c r="AG1" s="442" t="s">
+      <c r="AD1" s="452"/>
+      <c r="AE1" s="452"/>
+      <c r="AF1" s="453"/>
+      <c r="AG1" s="454" t="s">
         <v>14</v>
       </c>
-      <c r="AH1" s="443"/>
-      <c r="AI1" s="443"/>
-      <c r="AJ1" s="443"/>
-      <c r="AK1" s="442" t="s">
+      <c r="AH1" s="455"/>
+      <c r="AI1" s="455"/>
+      <c r="AJ1" s="455"/>
+      <c r="AK1" s="454" t="s">
         <v>68</v>
       </c>
-      <c r="AL1" s="443"/>
-      <c r="AM1" s="443"/>
-      <c r="AN1" s="443"/>
+      <c r="AL1" s="455"/>
+      <c r="AM1" s="455"/>
+      <c r="AN1" s="455"/>
     </row>
     <row r="2" spans="1:40" s="346" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="331" t="s">
@@ -16647,8 +16570,8 @@
       <c r="O8" s="348" t="s">
         <v>686</v>
       </c>
-      <c r="P8" s="452" t="s">
-        <v>1045</v>
+      <c r="P8" s="430" t="s">
+        <v>1042</v>
       </c>
       <c r="Q8" s="7">
         <v>1</v>
@@ -16725,8 +16648,8 @@
       <c r="O9" s="426" t="s">
         <v>688</v>
       </c>
-      <c r="P9" s="452" t="s">
-        <v>1046</v>
+      <c r="P9" s="430" t="s">
+        <v>1043</v>
       </c>
       <c r="Q9" s="7">
         <v>1</v>
@@ -16803,8 +16726,8 @@
       <c r="O10" s="394" t="s">
         <v>387</v>
       </c>
-      <c r="P10" s="452" t="s">
-        <v>1047</v>
+      <c r="P10" s="430" t="s">
+        <v>1044</v>
       </c>
       <c r="Q10" s="7">
         <v>1</v>
@@ -17202,7 +17125,7 @@
       <c r="S15" s="7"/>
       <c r="T15" s="7"/>
       <c r="U15" s="7" t="s">
-        <v>1044</v>
+        <v>1041</v>
       </c>
       <c r="V15" s="7"/>
       <c r="W15" s="355" t="s">
@@ -17237,75 +17160,75 @@
     <mergeCell ref="AK1:AN1"/>
   </mergeCells>
   <conditionalFormatting sqref="T1:T2 T16:T1048576">
-    <cfRule type="cellIs" dxfId="39" priority="54" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="54" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="56" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="56" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R1:S2 U11:V11 R13:V13 R16:S1048576 R4:T10 Q15:T15 Q8:R10">
-    <cfRule type="cellIs" dxfId="37" priority="55" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="55" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S3:T3">
-    <cfRule type="cellIs" dxfId="36" priority="47" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="47" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R3">
-    <cfRule type="cellIs" dxfId="35" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="46" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U12:V12">
-    <cfRule type="cellIs" dxfId="34" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="26" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q1:Q2 Q11 Q13 Q16:Q1048576">
-    <cfRule type="cellIs" dxfId="33" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="25" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q3">
-    <cfRule type="cellIs" dxfId="32" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="23" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q4">
-    <cfRule type="cellIs" dxfId="31" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="20" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q5">
-    <cfRule type="cellIs" dxfId="30" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="19" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q6:Q7">
-    <cfRule type="cellIs" dxfId="29" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="18" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q12">
-    <cfRule type="cellIs" dxfId="28" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="14" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R11:T12">
-    <cfRule type="cellIs" dxfId="27" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="12" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R14:V14">
-    <cfRule type="cellIs" dxfId="26" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="10" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q14">
-    <cfRule type="cellIs" dxfId="25" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="9" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17319,10 +17242,10 @@
   <dimension ref="A1:AM54"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="S12" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="K30" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="W13" sqref="W13"/>
+      <selection pane="bottomRight" activeCell="O33" sqref="O33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -17374,21 +17297,21 @@
       <c r="X1" s="69"/>
       <c r="Y1" s="70"/>
       <c r="Z1" s="70"/>
-      <c r="AA1" s="438" t="s">
+      <c r="AA1" s="450" t="s">
         <v>12</v>
       </c>
-      <c r="AB1" s="438"/>
-      <c r="AC1" s="438"/>
-      <c r="AD1" s="438" t="s">
+      <c r="AB1" s="450"/>
+      <c r="AC1" s="450"/>
+      <c r="AD1" s="450" t="s">
         <v>13</v>
       </c>
-      <c r="AE1" s="438"/>
-      <c r="AF1" s="438"/>
-      <c r="AG1" s="438" t="s">
+      <c r="AE1" s="450"/>
+      <c r="AF1" s="450"/>
+      <c r="AG1" s="450" t="s">
         <v>14</v>
       </c>
-      <c r="AH1" s="438"/>
-      <c r="AI1" s="438"/>
+      <c r="AH1" s="450"/>
+      <c r="AI1" s="450"/>
       <c r="AJ1" s="105" t="s">
         <v>136</v>
       </c>
@@ -17402,7 +17325,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="2" spans="1:39" s="25" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:39" s="25" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A2" s="255" t="s">
         <v>71</v>
       </c>
@@ -18203,7 +18126,7 @@
         <v>35</v>
       </c>
       <c r="B10" s="212" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("Indicatore ",C10," - ",D10)</f>
         <v>Indicatore 209 - XRA_SCONF_UTI_L1M</v>
       </c>
       <c r="C10" s="213">
@@ -18532,7 +18455,7 @@
       <c r="N13" s="100"/>
       <c r="O13" s="47"/>
       <c r="P13" s="47" t="s">
-        <v>1030</v>
+        <v>1027</v>
       </c>
       <c r="Q13" s="6">
         <v>2</v>
@@ -20079,7 +20002,7 @@
       <c r="O30" s="395" t="s">
         <v>773</v>
       </c>
-      <c r="P30" s="458" t="s">
+      <c r="P30" s="436" t="s">
         <v>773</v>
       </c>
       <c r="Q30" s="6">
@@ -20156,7 +20079,7 @@
       <c r="O31" s="372" t="s">
         <v>776</v>
       </c>
-      <c r="P31" s="459" t="s">
+      <c r="P31" s="437" t="s">
         <v>776</v>
       </c>
       <c r="Q31" s="6">
@@ -20233,8 +20156,8 @@
       <c r="O32" s="47" t="s">
         <v>774</v>
       </c>
-      <c r="P32" s="460" t="s">
-        <v>1031</v>
+      <c r="P32" s="438" t="s">
+        <v>1028</v>
       </c>
       <c r="Q32" s="6">
         <v>2</v>
@@ -20310,8 +20233,8 @@
       <c r="O33" s="189" t="s">
         <v>840</v>
       </c>
-      <c r="P33" s="459" t="s">
-        <v>1032</v>
+      <c r="P33" s="437" t="s">
+        <v>1029</v>
       </c>
       <c r="Q33" s="6">
         <v>2</v>
@@ -20620,8 +20543,8 @@
       <c r="O37" s="375" t="s">
         <v>834</v>
       </c>
-      <c r="P37" s="461" t="s">
-        <v>1033</v>
+      <c r="P37" s="439" t="s">
+        <v>1030</v>
       </c>
       <c r="Q37" s="6">
         <v>2</v>
@@ -20930,8 +20853,8 @@
       <c r="O41" s="374" t="s">
         <v>763</v>
       </c>
-      <c r="P41" s="461" t="s">
-        <v>1034</v>
+      <c r="P41" s="439" t="s">
+        <v>1031</v>
       </c>
       <c r="Q41" s="6">
         <v>2</v>
@@ -21005,8 +20928,8 @@
       <c r="O42" s="374" t="s">
         <v>836</v>
       </c>
-      <c r="P42" s="462" t="s">
-        <v>1035</v>
+      <c r="P42" s="440" t="s">
+        <v>1032</v>
       </c>
       <c r="Q42" s="6">
         <v>2</v>
@@ -21232,8 +21155,8 @@
       <c r="O45" s="375" t="s">
         <v>837</v>
       </c>
-      <c r="P45" s="461" t="s">
-        <v>1036</v>
+      <c r="P45" s="439" t="s">
+        <v>1033</v>
       </c>
       <c r="Q45" s="6">
         <v>2</v>
@@ -21386,8 +21309,8 @@
       <c r="O47" s="374" t="s">
         <v>838</v>
       </c>
-      <c r="P47" s="461" t="s">
-        <v>1037</v>
+      <c r="P47" s="439" t="s">
+        <v>1034</v>
       </c>
       <c r="Q47" s="6">
         <v>2</v>
@@ -21540,8 +21463,8 @@
       <c r="O49" s="374" t="s">
         <v>839</v>
       </c>
-      <c r="P49" s="461" t="s">
-        <v>1038</v>
+      <c r="P49" s="439" t="s">
+        <v>1035</v>
       </c>
       <c r="Q49" s="6">
         <v>2</v>
@@ -21767,8 +21690,8 @@
       <c r="O52" s="374" t="s">
         <v>928</v>
       </c>
-      <c r="P52" s="461" t="s">
-        <v>1039</v>
+      <c r="P52" s="439" t="s">
+        <v>1036</v>
       </c>
       <c r="Q52" s="6">
         <v>2</v>
@@ -21842,7 +21765,7 @@
       <c r="O53" s="401" t="s">
         <v>771</v>
       </c>
-      <c r="P53" s="463" t="s">
+      <c r="P53" s="441" t="s">
         <v>927</v>
       </c>
       <c r="Q53" s="6">
@@ -21955,45 +21878,45 @@
     <mergeCell ref="AG1:AI1"/>
   </mergeCells>
   <conditionalFormatting sqref="V1:V2 V55:V1048576">
-    <cfRule type="cellIs" dxfId="24" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="16" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="18" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R1:U2 Q5:V10 Q12:V12 Q14:V27 R3:V27 Q55:U1048576 Q1:Q27">
-    <cfRule type="cellIs" dxfId="22" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="17" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R11:V11">
-    <cfRule type="cellIs" dxfId="21" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="7" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V11">
-    <cfRule type="cellIs" dxfId="20" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="6" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q28:V29">
-    <cfRule type="cellIs" dxfId="19" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="5" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q13:V13">
-    <cfRule type="cellIs" dxfId="18" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="4" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q30:V54">
-    <cfRule type="cellIs" dxfId="17" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="3" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O41">
-    <cfRule type="cellIs" dxfId="16" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="1" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -22056,35 +21979,35 @@
       <c r="O1" s="27"/>
       <c r="V1" s="10"/>
       <c r="W1" s="10"/>
-      <c r="X1" s="433" t="s">
+      <c r="X1" s="445" t="s">
         <v>12</v>
       </c>
-      <c r="Y1" s="434"/>
-      <c r="Z1" s="434"/>
-      <c r="AA1" s="435"/>
-      <c r="AB1" s="433" t="s">
+      <c r="Y1" s="446"/>
+      <c r="Z1" s="446"/>
+      <c r="AA1" s="447"/>
+      <c r="AB1" s="445" t="s">
         <v>13</v>
       </c>
-      <c r="AC1" s="434"/>
-      <c r="AD1" s="434"/>
-      <c r="AE1" s="435"/>
-      <c r="AF1" s="436" t="s">
+      <c r="AC1" s="446"/>
+      <c r="AD1" s="446"/>
+      <c r="AE1" s="447"/>
+      <c r="AF1" s="448" t="s">
         <v>14</v>
       </c>
-      <c r="AG1" s="437"/>
-      <c r="AH1" s="437"/>
-      <c r="AI1" s="437"/>
-      <c r="AJ1" s="436" t="s">
+      <c r="AG1" s="449"/>
+      <c r="AH1" s="449"/>
+      <c r="AI1" s="449"/>
+      <c r="AJ1" s="448" t="s">
         <v>68</v>
       </c>
-      <c r="AK1" s="437"/>
-      <c r="AL1" s="437"/>
-      <c r="AM1" s="437"/>
+      <c r="AK1" s="449"/>
+      <c r="AL1" s="449"/>
+      <c r="AM1" s="449"/>
       <c r="AN1" s="38"/>
-      <c r="AO1" s="444" t="s">
+      <c r="AO1" s="456" t="s">
         <v>20</v>
       </c>
-      <c r="AP1" s="444"/>
+      <c r="AP1" s="456"/>
     </row>
     <row r="2" spans="1:42" s="46" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A2" s="44" t="s">
@@ -22224,20 +22147,20 @@
     <mergeCell ref="AO1:AP1"/>
   </mergeCells>
   <conditionalFormatting sqref="S1:S1048576">
-    <cfRule type="cellIs" dxfId="15" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="21" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="23" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q1:R1048576">
-    <cfRule type="cellIs" dxfId="13" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="22" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P1:P1048576">
-    <cfRule type="cellIs" dxfId="12" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="17" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -22998,55 +22921,55 @@
     <sortCondition ref="C2"/>
   </sortState>
   <conditionalFormatting sqref="W1">
-    <cfRule type="cellIs" dxfId="11" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="13" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="15" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U1:V1">
-    <cfRule type="cellIs" dxfId="9" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="14" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U2:V3">
-    <cfRule type="cellIs" dxfId="8" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="12" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W2:W3">
-    <cfRule type="cellIs" dxfId="7" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="11" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U4:V4">
-    <cfRule type="cellIs" dxfId="6" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="10" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W4">
-    <cfRule type="cellIs" dxfId="5" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U5:V5">
-    <cfRule type="cellIs" dxfId="4" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="8" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W5">
-    <cfRule type="cellIs" dxfId="3" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U6:V7">
-    <cfRule type="cellIs" dxfId="2" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W6:W7">
-    <cfRule type="cellIs" dxfId="1" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -23059,8 +22982,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="A52" sqref="A52"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -23128,8 +23051,8 @@
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A6" s="453" t="s">
-        <v>968</v>
+      <c r="A6" s="431" t="s">
+        <v>965</v>
       </c>
       <c r="B6" t="s">
         <v>72</v>
@@ -23151,8 +23074,8 @@
       <c r="I6" s="193"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A7" s="453" t="s">
-        <v>969</v>
+      <c r="A7" s="431" t="s">
+        <v>966</v>
       </c>
       <c r="B7" t="s">
         <v>72</v>
@@ -23174,8 +23097,8 @@
       <c r="I7" s="193"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A8" s="453" t="s">
-        <v>970</v>
+      <c r="A8" s="431" t="s">
+        <v>967</v>
       </c>
       <c r="B8" t="s">
         <v>72</v>
@@ -23197,8 +23120,8 @@
       <c r="I8" s="193"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A9" s="453" t="s">
-        <v>971</v>
+      <c r="A9" s="431" t="s">
+        <v>968</v>
       </c>
       <c r="B9" t="s">
         <v>72</v>
@@ -23220,8 +23143,8 @@
       <c r="I9" s="193"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A10" s="453" t="s">
-        <v>972</v>
+      <c r="A10" s="431" t="s">
+        <v>969</v>
       </c>
       <c r="B10" t="s">
         <v>72</v>
@@ -23243,8 +23166,8 @@
       <c r="I10" s="193"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A11" s="453" t="s">
-        <v>973</v>
+      <c r="A11" s="431" t="s">
+        <v>970</v>
       </c>
       <c r="B11" t="s">
         <v>72</v>
@@ -23256,14 +23179,14 @@
         <v>429</v>
       </c>
       <c r="E11" s="420" t="s">
-        <v>967</v>
+        <v>964</v>
       </c>
       <c r="F11" s="419"/>
       <c r="G11"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A12" s="453" t="s">
-        <v>974</v>
+      <c r="A12" s="431" t="s">
+        <v>971</v>
       </c>
       <c r="B12" t="s">
         <v>72</v>
@@ -23275,14 +23198,14 @@
         <v>429</v>
       </c>
       <c r="E12" s="421" t="s">
-        <v>964</v>
+        <v>961</v>
       </c>
       <c r="F12" s="419"/>
       <c r="G12"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A13" s="453" t="s">
-        <v>975</v>
+      <c r="A13" s="431" t="s">
+        <v>972</v>
       </c>
       <c r="B13" t="s">
         <v>72</v>
@@ -23294,14 +23217,14 @@
         <v>429</v>
       </c>
       <c r="E13" s="421" t="s">
-        <v>963</v>
+        <v>960</v>
       </c>
       <c r="F13" s="419"/>
       <c r="G13"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A14" s="453" t="s">
-        <v>976</v>
+      <c r="A14" s="431" t="s">
+        <v>973</v>
       </c>
       <c r="B14" t="s">
         <v>72</v>
@@ -23313,14 +23236,14 @@
         <v>429</v>
       </c>
       <c r="E14" s="421" t="s">
-        <v>962</v>
+        <v>959</v>
       </c>
       <c r="F14" s="419"/>
       <c r="G14"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A15" s="453" t="s">
-        <v>977</v>
+      <c r="A15" s="431" t="s">
+        <v>974</v>
       </c>
       <c r="B15" t="s">
         <v>72</v>
@@ -23332,14 +23255,14 @@
         <v>429</v>
       </c>
       <c r="E15" s="422" t="s">
-        <v>961</v>
+        <v>958</v>
       </c>
       <c r="F15" s="419"/>
       <c r="G15"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A16" s="453" t="s">
-        <v>978</v>
+      <c r="A16" s="431" t="s">
+        <v>975</v>
       </c>
       <c r="B16" t="s">
         <v>72</v>
@@ -23351,14 +23274,14 @@
         <v>429</v>
       </c>
       <c r="E16" s="420" t="s">
-        <v>957</v>
+        <v>954</v>
       </c>
       <c r="F16" s="419"/>
       <c r="G16"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" s="453" t="s">
-        <v>993</v>
+      <c r="A17" s="431" t="s">
+        <v>990</v>
       </c>
       <c r="B17" t="s">
         <v>72</v>
@@ -23370,7 +23293,7 @@
         <v>429</v>
       </c>
       <c r="E17" s="193" t="s">
-        <v>965</v>
+        <v>962</v>
       </c>
       <c r="F17" s="221"/>
       <c r="G17" s="222" t="s">
@@ -23380,8 +23303,8 @@
       <c r="I17" s="193"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" s="453" t="s">
-        <v>979</v>
+      <c r="A18" s="431" t="s">
+        <v>976</v>
       </c>
       <c r="B18" t="s">
         <v>72</v>
@@ -23403,8 +23326,8 @@
       <c r="I18" s="193"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="453" t="s">
-        <v>980</v>
+      <c r="A19" s="431" t="s">
+        <v>977</v>
       </c>
       <c r="B19" t="s">
         <v>72</v>
@@ -23426,8 +23349,8 @@
       <c r="I19" s="193"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A20" s="453" t="s">
-        <v>981</v>
+      <c r="A20" s="431" t="s">
+        <v>978</v>
       </c>
       <c r="B20" t="s">
         <v>72</v>
@@ -23449,8 +23372,8 @@
       <c r="I20" s="193"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A21" s="453" t="s">
-        <v>982</v>
+      <c r="A21" s="431" t="s">
+        <v>979</v>
       </c>
       <c r="B21" t="s">
         <v>72</v>
@@ -23472,8 +23395,8 @@
       <c r="I21" s="193"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A22" s="453" t="s">
-        <v>983</v>
+      <c r="A22" s="431" t="s">
+        <v>980</v>
       </c>
       <c r="B22" t="s">
         <v>72</v>
@@ -23495,8 +23418,8 @@
       <c r="I22" s="193"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A23" s="453" t="s">
-        <v>984</v>
+      <c r="A23" s="431" t="s">
+        <v>981</v>
       </c>
       <c r="B23" t="s">
         <v>72</v>
@@ -23518,8 +23441,8 @@
       <c r="I23" s="193"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A24" s="453" t="s">
-        <v>985</v>
+      <c r="A24" s="431" t="s">
+        <v>982</v>
       </c>
       <c r="B24" t="s">
         <v>72</v>
@@ -23531,14 +23454,14 @@
         <v>429</v>
       </c>
       <c r="E24" s="420" t="s">
-        <v>958</v>
+        <v>955</v>
       </c>
       <c r="F24" s="419"/>
       <c r="G24"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A25" s="453" t="s">
-        <v>986</v>
+      <c r="A25" s="431" t="s">
+        <v>983</v>
       </c>
       <c r="B25" t="s">
         <v>72</v>
@@ -23560,8 +23483,8 @@
       <c r="I25" s="193"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A26" s="453" t="s">
-        <v>987</v>
+      <c r="A26" s="431" t="s">
+        <v>984</v>
       </c>
       <c r="B26" t="s">
         <v>72</v>
@@ -23583,8 +23506,8 @@
       <c r="I26" s="193"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A27" s="453" t="s">
-        <v>988</v>
+      <c r="A27" s="431" t="s">
+        <v>985</v>
       </c>
       <c r="B27" t="s">
         <v>72</v>
@@ -23606,8 +23529,8 @@
       <c r="I27" s="193"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A28" s="453" t="s">
-        <v>989</v>
+      <c r="A28" s="431" t="s">
+        <v>986</v>
       </c>
       <c r="B28" t="s">
         <v>72</v>
@@ -23629,8 +23552,8 @@
       <c r="I28" s="193"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A29" s="453" t="s">
-        <v>990</v>
+      <c r="A29" s="431" t="s">
+        <v>987</v>
       </c>
       <c r="B29" t="s">
         <v>72</v>
@@ -23642,14 +23565,14 @@
         <v>429</v>
       </c>
       <c r="E29" s="420" t="s">
-        <v>959</v>
+        <v>956</v>
       </c>
       <c r="F29" s="419"/>
       <c r="G29"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A30" s="453" t="s">
-        <v>991</v>
+      <c r="A30" s="431" t="s">
+        <v>988</v>
       </c>
       <c r="B30" t="s">
         <v>72</v>
@@ -23671,8 +23594,8 @@
       <c r="I30" s="193"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A31" s="453" t="s">
-        <v>992</v>
+      <c r="A31" s="431" t="s">
+        <v>989</v>
       </c>
       <c r="B31" t="s">
         <v>72</v>
@@ -23684,14 +23607,14 @@
         <v>429</v>
       </c>
       <c r="E31" s="422" t="s">
-        <v>960</v>
+        <v>957</v>
       </c>
       <c r="F31" s="419"/>
       <c r="G31"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A32" s="453" t="s">
-        <v>1027</v>
+      <c r="A32" s="431" t="s">
+        <v>1024</v>
       </c>
       <c r="B32" t="s">
         <v>72</v>
@@ -23703,14 +23626,14 @@
         <v>429</v>
       </c>
       <c r="E32" s="422" t="s">
-        <v>1026</v>
+        <v>1023</v>
       </c>
       <c r="F32" s="419"/>
       <c r="G32"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A33" s="453" t="s">
-        <v>994</v>
+      <c r="A33" s="431" t="s">
+        <v>991</v>
       </c>
       <c r="B33" t="s">
         <v>72</v>
@@ -23732,8 +23655,8 @@
       <c r="I33" s="193"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A34" s="453" t="s">
-        <v>995</v>
+      <c r="A34" s="431" t="s">
+        <v>992</v>
       </c>
       <c r="B34" t="s">
         <v>72</v>
@@ -23755,8 +23678,8 @@
       <c r="I34" s="193"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A35" s="456" t="s">
-        <v>1040</v>
+      <c r="A35" s="434" t="s">
+        <v>1037</v>
       </c>
       <c r="B35" t="s">
         <v>72</v>
@@ -23768,12 +23691,12 @@
         <v>413</v>
       </c>
       <c r="E35" s="193" t="s">
-        <v>1041</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A36" s="457" t="s">
-        <v>1042</v>
+      <c r="A36" s="435" t="s">
+        <v>1039</v>
       </c>
       <c r="B36" t="s">
         <v>72</v>
@@ -23785,12 +23708,12 @@
         <v>413</v>
       </c>
       <c r="E36" s="193" t="s">
-        <v>1043</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A37" s="453" t="s">
-        <v>996</v>
+      <c r="A37" s="431" t="s">
+        <v>993</v>
       </c>
       <c r="B37" t="s">
         <v>931</v>
@@ -23812,8 +23735,8 @@
       <c r="I37" s="193"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A38" s="453" t="s">
-        <v>997</v>
+      <c r="A38" s="431" t="s">
+        <v>994</v>
       </c>
       <c r="B38" t="s">
         <v>931</v>
@@ -23835,8 +23758,8 @@
       <c r="I38" s="193"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A39" s="454" t="s">
-        <v>1006</v>
+      <c r="A39" s="432" t="s">
+        <v>1003</v>
       </c>
       <c r="B39" s="412" t="s">
         <v>532</v>
@@ -23848,15 +23771,15 @@
         <v>413</v>
       </c>
       <c r="E39" s="414" t="s">
-        <v>946</v>
+        <v>943</v>
       </c>
       <c r="G39" s="222" t="s">
         <v>417</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A40" s="454" t="s">
-        <v>1007</v>
+      <c r="A40" s="432" t="s">
+        <v>1004</v>
       </c>
       <c r="B40" s="412" t="s">
         <v>532</v>
@@ -23867,19 +23790,19 @@
       <c r="D40" s="413" t="s">
         <v>414</v>
       </c>
-      <c r="E40" s="414" t="s">
-        <v>945</v>
+      <c r="E40" s="464" t="s">
+        <v>1050</v>
       </c>
       <c r="G40" s="222" t="s">
         <v>417</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A41" s="454" t="s">
-        <v>1011</v>
+      <c r="A41" s="432" t="s">
+        <v>1008</v>
       </c>
       <c r="B41" s="412" t="s">
-        <v>950</v>
+        <v>947</v>
       </c>
       <c r="C41" s="412" t="s">
         <v>935</v>
@@ -23888,18 +23811,18 @@
         <v>413</v>
       </c>
       <c r="E41" s="414" t="s">
-        <v>953</v>
+        <v>950</v>
       </c>
       <c r="G41" s="222" t="s">
         <v>417</v>
       </c>
     </row>
     <row r="42" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="454" t="s">
-        <v>1012</v>
+      <c r="A42" s="432" t="s">
+        <v>1009</v>
       </c>
       <c r="B42" s="412" t="s">
-        <v>950</v>
+        <v>947</v>
       </c>
       <c r="C42" s="412" t="s">
         <v>935</v>
@@ -23908,18 +23831,18 @@
         <v>414</v>
       </c>
       <c r="E42" s="414" t="s">
-        <v>951</v>
+        <v>948</v>
       </c>
       <c r="G42" s="222" t="s">
         <v>417</v>
       </c>
     </row>
     <row r="43" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="454" t="s">
-        <v>1013</v>
+      <c r="A43" s="432" t="s">
+        <v>1010</v>
       </c>
       <c r="B43" s="412" t="s">
-        <v>950</v>
+        <v>947</v>
       </c>
       <c r="C43" s="412" t="s">
         <v>935</v>
@@ -23928,15 +23851,15 @@
         <v>414</v>
       </c>
       <c r="E43" s="414" t="s">
-        <v>952</v>
+        <v>949</v>
       </c>
       <c r="G43" s="222" t="s">
         <v>417</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A44" s="454" t="s">
-        <v>998</v>
+      <c r="A44" s="432" t="s">
+        <v>995</v>
       </c>
       <c r="B44" s="412" t="s">
         <v>934</v>
@@ -23948,7 +23871,7 @@
         <v>413</v>
       </c>
       <c r="E44" s="414" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="G44" s="222" t="s">
         <v>417</v>
@@ -23957,8 +23880,8 @@
       <c r="I44" s="193"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A45" s="454" t="s">
-        <v>999</v>
+      <c r="A45" s="432" t="s">
+        <v>996</v>
       </c>
       <c r="B45" s="412" t="s">
         <v>934</v>
@@ -23969,8 +23892,8 @@
       <c r="D45" s="413" t="s">
         <v>414</v>
       </c>
-      <c r="E45" s="414" t="s">
-        <v>936</v>
+      <c r="E45" s="464" t="s">
+        <v>1048</v>
       </c>
       <c r="G45" s="222" t="s">
         <v>417</v>
@@ -23979,8 +23902,8 @@
       <c r="I45" s="193"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A46" s="454" t="s">
-        <v>1000</v>
+      <c r="A46" s="432" t="s">
+        <v>997</v>
       </c>
       <c r="B46" s="412" t="s">
         <v>934</v>
@@ -23992,14 +23915,14 @@
         <v>415</v>
       </c>
       <c r="E46" s="414" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="H46" s="193"/>
       <c r="I46" s="107"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A47" s="454" t="s">
-        <v>1001</v>
+      <c r="A47" s="432" t="s">
+        <v>998</v>
       </c>
       <c r="B47" s="412" t="s">
         <v>934</v>
@@ -24011,17 +23934,17 @@
         <v>430</v>
       </c>
       <c r="E47" s="427" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="H47" s="193"/>
       <c r="I47" s="193"/>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A48" s="454" t="s">
-        <v>1002</v>
+      <c r="A48" s="432" t="s">
+        <v>999</v>
       </c>
       <c r="B48" s="412" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="C48" s="412" t="s">
         <v>935</v>
@@ -24030,18 +23953,18 @@
         <v>413</v>
       </c>
       <c r="E48" s="414" t="s">
-        <v>942</v>
+        <v>940</v>
       </c>
       <c r="G48" s="222" t="s">
         <v>417</v>
       </c>
     </row>
     <row r="49" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="454" t="s">
-        <v>1003</v>
+      <c r="A49" s="432" t="s">
+        <v>1000</v>
       </c>
       <c r="B49" s="412" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="C49" s="412" t="s">
         <v>935</v>
@@ -24049,19 +23972,19 @@
       <c r="D49" s="413" t="s">
         <v>414</v>
       </c>
-      <c r="E49" s="414" t="s">
-        <v>941</v>
+      <c r="E49" s="464" t="s">
+        <v>1049</v>
       </c>
       <c r="G49" s="222" t="s">
         <v>417</v>
       </c>
     </row>
     <row r="50" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="454" t="s">
-        <v>1004</v>
+      <c r="A50" s="432" t="s">
+        <v>1001</v>
       </c>
       <c r="B50" s="412" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="C50" s="412" t="s">
         <v>935</v>
@@ -24070,15 +23993,15 @@
         <v>415</v>
       </c>
       <c r="E50" s="414" t="s">
-        <v>943</v>
+        <v>941</v>
       </c>
     </row>
     <row r="51" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="454" t="s">
-        <v>1005</v>
+      <c r="A51" s="432" t="s">
+        <v>1002</v>
       </c>
       <c r="B51" s="412" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="C51" s="412" t="s">
         <v>935</v>
@@ -24087,12 +24010,12 @@
         <v>430</v>
       </c>
       <c r="E51" s="428" t="s">
-        <v>944</v>
+        <v>942</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A52" s="454" t="s">
-        <v>1008</v>
+      <c r="A52" s="432" t="s">
+        <v>1005</v>
       </c>
       <c r="B52" s="412" t="s">
         <v>361</v>
@@ -24104,15 +24027,15 @@
         <v>414</v>
       </c>
       <c r="E52" s="414" t="s">
-        <v>947</v>
+        <v>944</v>
       </c>
       <c r="G52" s="222" t="s">
         <v>417</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A53" s="454" t="s">
-        <v>1009</v>
+      <c r="A53" s="432" t="s">
+        <v>1006</v>
       </c>
       <c r="B53" s="412" t="s">
         <v>361</v>
@@ -24124,12 +24047,12 @@
         <v>415</v>
       </c>
       <c r="E53" s="414" t="s">
-        <v>948</v>
+        <v>945</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A54" s="454" t="s">
-        <v>1010</v>
+      <c r="A54" s="432" t="s">
+        <v>1007</v>
       </c>
       <c r="B54" s="412" t="s">
         <v>361</v>
@@ -24141,12 +24064,12 @@
         <v>430</v>
       </c>
       <c r="E54" s="428" t="s">
-        <v>949</v>
+        <v>946</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A55" s="454" t="s">
-        <v>1014</v>
+      <c r="A55" s="432" t="s">
+        <v>1011</v>
       </c>
       <c r="B55" s="412" t="s">
         <v>570</v>
@@ -24158,15 +24081,15 @@
         <v>413</v>
       </c>
       <c r="E55" s="414" t="s">
-        <v>955</v>
+        <v>952</v>
       </c>
       <c r="G55" s="222" t="s">
         <v>417</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A56" s="454" t="s">
-        <v>1015</v>
+      <c r="A56" s="432" t="s">
+        <v>1012</v>
       </c>
       <c r="B56" s="412" t="s">
         <v>570</v>
@@ -24178,15 +24101,15 @@
         <v>414</v>
       </c>
       <c r="E56" s="428" t="s">
-        <v>954</v>
+        <v>951</v>
       </c>
       <c r="G56" s="222" t="s">
         <v>417</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A57" s="453" t="s">
-        <v>1025</v>
+      <c r="A57" s="431" t="s">
+        <v>1022</v>
       </c>
       <c r="B57" t="s">
         <v>747</v>
@@ -24208,8 +24131,8 @@
       <c r="I57" s="193"/>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A58" s="453" t="s">
-        <v>1016</v>
+      <c r="A58" s="431" t="s">
+        <v>1013</v>
       </c>
       <c r="B58" t="s">
         <v>259</v>
@@ -24231,8 +24154,8 @@
       <c r="I58" s="193"/>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A59" s="453" t="s">
-        <v>1017</v>
+      <c r="A59" s="431" t="s">
+        <v>1014</v>
       </c>
       <c r="B59" t="s">
         <v>259</v>
@@ -24254,8 +24177,8 @@
       <c r="I59" s="193"/>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A60" s="455" t="s">
-        <v>1018</v>
+      <c r="A60" s="433" t="s">
+        <v>1015</v>
       </c>
       <c r="B60" s="425" t="s">
         <v>259</v>
@@ -24279,8 +24202,8 @@
       <c r="I60" s="193"/>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A61" s="453" t="s">
-        <v>1023</v>
+      <c r="A61" s="431" t="s">
+        <v>1020</v>
       </c>
       <c r="B61" t="s">
         <v>266</v>
@@ -24300,8 +24223,8 @@
       <c r="I61" s="193"/>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A62" s="453" t="s">
-        <v>1024</v>
+      <c r="A62" s="431" t="s">
+        <v>1021</v>
       </c>
       <c r="B62" t="s">
         <v>933</v>
@@ -24323,8 +24246,8 @@
       <c r="I62" s="193"/>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A63" s="453" t="s">
-        <v>1019</v>
+      <c r="A63" s="431" t="s">
+        <v>1016</v>
       </c>
       <c r="B63" t="s">
         <v>932</v>
@@ -24344,8 +24267,8 @@
       <c r="I63" s="193"/>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A64" s="453" t="s">
-        <v>1020</v>
+      <c r="A64" s="431" t="s">
+        <v>1017</v>
       </c>
       <c r="B64" t="s">
         <v>932</v>
@@ -24365,8 +24288,8 @@
       <c r="I64" s="193"/>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A65" s="453" t="s">
-        <v>1021</v>
+      <c r="A65" s="431" t="s">
+        <v>1018</v>
       </c>
       <c r="B65" t="s">
         <v>932</v>
@@ -24378,18 +24301,18 @@
         <v>413</v>
       </c>
       <c r="E65" s="193" t="s">
-        <v>956</v>
+        <v>953</v>
       </c>
       <c r="F65" s="221" t="s">
-        <v>1028</v>
+        <v>1025</v>
       </c>
       <c r="G65" s="222"/>
       <c r="H65" s="193"/>
       <c r="I65" s="193"/>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A66" s="453" t="s">
-        <v>1022</v>
+      <c r="A66" s="431" t="s">
+        <v>1019</v>
       </c>
       <c r="B66" t="s">
         <v>932</v>
@@ -24414,11 +24337,11 @@
   <sortState ref="A6:I66">
     <sortCondition ref="C6:C66" customList="High Priority,Carta Commerciale,Preammortamenti,Qualitativo"/>
     <sortCondition ref="B6:B66" customList="High Priority"/>
-    <sortCondition sortBy="cellColor" ref="D6:D66" dxfId="95"/>
-    <sortCondition sortBy="cellColor" ref="D6:D66" dxfId="94"/>
-    <sortCondition sortBy="cellColor" ref="D6:D66" dxfId="93"/>
-    <sortCondition sortBy="cellColor" ref="D6:D66" dxfId="92"/>
-    <sortCondition sortBy="cellColor" ref="D6:D66" dxfId="91"/>
+    <sortCondition sortBy="cellColor" ref="D6:D66" dxfId="4"/>
+    <sortCondition sortBy="cellColor" ref="D6:D66" dxfId="3"/>
+    <sortCondition sortBy="cellColor" ref="D6:D66" dxfId="2"/>
+    <sortCondition sortBy="cellColor" ref="D6:D66" dxfId="1"/>
+    <sortCondition sortBy="cellColor" ref="D6:D66" dxfId="0"/>
     <sortCondition ref="A6:A66"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -24430,7 +24353,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3:E16"/>
     </sheetView>
   </sheetViews>
@@ -24465,7 +24388,7 @@
         <v>724</v>
       </c>
       <c r="D3" s="368" t="s">
-        <v>1048</v>
+        <v>1045</v>
       </c>
       <c r="E3" s="369" t="s">
         <v>739</v>
@@ -24519,7 +24442,7 @@
         <v>728</v>
       </c>
       <c r="D7" s="368" t="s">
-        <v>1049</v>
+        <v>1046</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -24576,7 +24499,7 @@
     <row r="16" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16"/>
       <c r="C16" s="366" t="s">
-        <v>1050</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -24708,18 +24631,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -24837,6 +24760,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C69AF5A-C63E-4E3E-821D-D66D815E3725}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{53FC0B01-7E98-4633-A4D4-301D890C7458}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
@@ -24847,14 +24778,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C69AF5A-C63E-4E3E-821D-D66D815E3725}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
afu e soglie sme
</commit_message>
<xml_diff>
--- a/earlywarning-pom/Document/SpecificheIndicatori/20161019 Indicatori EWS - Banche Italiane_SME_RETAIL.xlsx
+++ b/earlywarning-pom/Document/SpecificheIndicatori/20161019 Indicatori EWS - Banche Italiane_SME_RETAIL.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\michele.dessi\Desktop\AAAP\INTESA\Repository\client-intesa\earlywarning-pom\Document\SpecificheIndicatori\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ilaria.cutano\Desktop\ISP\git\client-intesa\client-intesa\earlywarning-pom\Document\SpecificheIndicatori\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="31995" windowHeight="16275" tabRatio="918" firstSheet="2" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="468" windowWidth="31992" windowHeight="16272" tabRatio="918" firstSheet="2" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Legenda" sheetId="20" r:id="rId1"/>
@@ -3794,9 +3794,6 @@
     <t>Carta Commerciale</t>
   </si>
   <si>
-    <t>IND_164 &lt; 0.20 AND IND_165 &gt; 30</t>
-  </si>
-  <si>
     <t>IND_164 &gt;= 0.20 AND IND_165 &gt; 30</t>
   </si>
   <si>
@@ -3807,9 +3804,6 @@
   </si>
   <si>
     <t>Finanziamenti esteri - Finimport</t>
-  </si>
-  <si>
-    <t>IND_166 &lt; 0.20 AND IND_167 &gt; 30</t>
   </si>
   <si>
     <t>IND_166 &gt;= 0.20 AND IND_167 &gt; 30</t>
@@ -4392,6 +4386,12 @@
   </si>
   <si>
     <t>L'indicatore riporta, per la controparte oggetto di valutazione EW, l'importo residuo sconfinato (anche parziali) per i prodotti rateali con addebito diretto su c/c Banca (ISP o CLONE).</t>
+  </si>
+  <si>
+    <t>0,05&lt;= IND_164 &lt; 0.20 AND IND_165 &gt; 30</t>
+  </si>
+  <si>
+    <t>0,05 &lt;= IND_166 &lt; 0.20 AND IND_167 &gt; 30</t>
   </si>
 </sst>
 </file>
@@ -6670,6 +6670,12 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -6735,23 +6741,17 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="Bad 2" xfId="2"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="7" builtinId="8"/>
     <cellStyle name="Normal 2" xfId="1"/>
     <cellStyle name="Normal 3" xfId="3"/>
     <cellStyle name="Normal 4" xfId="4"/>
     <cellStyle name="Normal 4 2" xfId="6"/>
     <cellStyle name="Normal 5" xfId="5"/>
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="85">
     <dxf>
@@ -7886,33 +7886,33 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.125" customWidth="1"/>
-    <col min="2" max="2" width="8.875" style="45"/>
-    <col min="3" max="3" width="29.875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.625" customWidth="1"/>
-    <col min="5" max="5" width="6.375" customWidth="1"/>
+    <col min="1" max="1" width="2.09765625" customWidth="1"/>
+    <col min="2" max="2" width="8.8984375" style="45"/>
+    <col min="3" max="3" width="29.8984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.59765625" customWidth="1"/>
+    <col min="5" max="5" width="6.3984375" customWidth="1"/>
     <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.25" customWidth="1"/>
-    <col min="8" max="8" width="4.75" style="229" customWidth="1"/>
-    <col min="9" max="9" width="40.125" style="229" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.19921875" customWidth="1"/>
+    <col min="8" max="8" width="4.69921875" style="229" customWidth="1"/>
+    <col min="9" max="9" width="40.09765625" style="229" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9.5" style="228" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.3984375" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="11" bestFit="1" customWidth="1"/>
-    <col min="15" max="18" width="10.75" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.25" bestFit="1" customWidth="1"/>
+    <col min="15" max="18" width="10.69921875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.19921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="E1" s="428" t="s">
+    <row r="1" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="E1" s="430" t="s">
         <v>420</v>
       </c>
-      <c r="F1" s="428"/>
-      <c r="H1" s="429" t="s">
+      <c r="F1" s="430"/>
+      <c r="H1" s="431" t="s">
         <v>256</v>
       </c>
-      <c r="I1" s="430"/>
+      <c r="I1" s="432"/>
       <c r="J1" t="s">
         <v>251</v>
       </c>
@@ -7938,7 +7938,7 @@
         <v>766</v>
       </c>
     </row>
-    <row r="2" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B2" s="206"/>
       <c r="C2" t="s">
         <v>371</v>
@@ -7984,7 +7984,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B3" s="204"/>
       <c r="C3" s="203" t="s">
         <v>301</v>
@@ -8030,7 +8030,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B4" s="205"/>
       <c r="C4" s="203" t="s">
         <v>302</v>
@@ -8076,7 +8076,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B5" s="207"/>
       <c r="C5" t="s">
         <v>322</v>
@@ -8122,7 +8122,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B6" s="213"/>
       <c r="C6" t="s">
         <v>354</v>
@@ -8149,7 +8149,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="7" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B7" s="209"/>
       <c r="C7" t="s">
         <v>323</v>
@@ -8191,7 +8191,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="8" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B8" s="215" t="s">
         <v>374</v>
       </c>
@@ -8235,7 +8235,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="9" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B9" s="233"/>
       <c r="C9" t="s">
         <v>478</v>
@@ -8271,7 +8271,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="10" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:18" x14ac:dyDescent="0.3">
       <c r="H10" s="232" t="s">
         <v>438</v>
       </c>
@@ -8303,7 +8303,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:18" x14ac:dyDescent="0.3">
       <c r="H11" s="232" t="s">
         <v>440</v>
       </c>
@@ -8320,7 +8320,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="12" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:18" x14ac:dyDescent="0.3">
       <c r="H12" s="232" t="s">
         <v>442</v>
       </c>
@@ -8356,7 +8356,7 @@
         <v>1.375</v>
       </c>
     </row>
-    <row r="13" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B13" s="261"/>
       <c r="C13" t="s">
         <v>612</v>
@@ -8396,7 +8396,7 @@
         <v>4.25</v>
       </c>
     </row>
-    <row r="14" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B14" s="262"/>
       <c r="C14" t="s">
         <v>613</v>
@@ -8436,7 +8436,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B15" s="263"/>
       <c r="C15" t="s">
         <v>614</v>
@@ -8476,7 +8476,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:18" x14ac:dyDescent="0.3">
       <c r="H16" s="232" t="s">
         <v>450</v>
       </c>
@@ -8512,7 +8512,7 @@
         <v>20.625</v>
       </c>
     </row>
-    <row r="17" spans="8:19" x14ac:dyDescent="0.25">
+    <row r="17" spans="8:19" x14ac:dyDescent="0.3">
       <c r="H17" s="232" t="s">
         <v>452</v>
       </c>
@@ -8529,7 +8529,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="18" spans="8:19" x14ac:dyDescent="0.25">
+    <row r="18" spans="8:19" x14ac:dyDescent="0.3">
       <c r="H18" s="232" t="s">
         <v>454</v>
       </c>
@@ -8564,7 +8564,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="19" spans="8:19" x14ac:dyDescent="0.25">
+    <row r="19" spans="8:19" x14ac:dyDescent="0.3">
       <c r="H19" s="232" t="s">
         <v>456</v>
       </c>
@@ -8595,7 +8595,7 @@
       </c>
       <c r="S19" s="135"/>
     </row>
-    <row r="20" spans="8:19" x14ac:dyDescent="0.25">
+    <row r="20" spans="8:19" x14ac:dyDescent="0.3">
       <c r="H20" s="232" t="s">
         <v>458</v>
       </c>
@@ -8622,7 +8622,7 @@
       </c>
       <c r="S20" s="135"/>
     </row>
-    <row r="21" spans="8:19" x14ac:dyDescent="0.25">
+    <row r="21" spans="8:19" x14ac:dyDescent="0.3">
       <c r="H21" s="232" t="s">
         <v>460</v>
       </c>
@@ -8647,7 +8647,7 @@
       </c>
       <c r="S21" s="135"/>
     </row>
-    <row r="22" spans="8:19" x14ac:dyDescent="0.25">
+    <row r="22" spans="8:19" x14ac:dyDescent="0.3">
       <c r="H22" s="232" t="s">
         <v>462</v>
       </c>
@@ -8672,7 +8672,7 @@
       </c>
       <c r="S22" s="135"/>
     </row>
-    <row r="23" spans="8:19" x14ac:dyDescent="0.25">
+    <row r="23" spans="8:19" x14ac:dyDescent="0.3">
       <c r="H23" s="232" t="s">
         <v>483</v>
       </c>
@@ -8685,7 +8685,7 @@
       </c>
       <c r="L23" s="192"/>
       <c r="N23" s="135" t="s">
-        <v>942</v>
+        <v>940</v>
       </c>
       <c r="O23" s="135"/>
       <c r="P23" s="135" t="s">
@@ -8695,7 +8695,7 @@
       <c r="R23" s="135"/>
       <c r="S23" s="135"/>
     </row>
-    <row r="24" spans="8:19" x14ac:dyDescent="0.25">
+    <row r="24" spans="8:19" x14ac:dyDescent="0.3">
       <c r="H24" s="232" t="s">
         <v>485</v>
       </c>
@@ -8718,7 +8718,7 @@
       <c r="R24" s="135"/>
       <c r="S24" s="135"/>
     </row>
-    <row r="25" spans="8:19" x14ac:dyDescent="0.25">
+    <row r="25" spans="8:19" x14ac:dyDescent="0.3">
       <c r="N25" s="135" t="s">
         <v>773</v>
       </c>
@@ -8748,21 +8748,21 @@
       <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="47.625" customWidth="1"/>
-    <col min="4" max="4" width="16.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="47.59765625" customWidth="1"/>
+    <col min="4" max="4" width="16.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F1" s="447" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F1" s="449" t="s">
         <v>176</v>
       </c>
-      <c r="G1" s="447"/>
-      <c r="H1" s="447"/>
-    </row>
-    <row r="2" spans="1:8" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G1" s="449"/>
+      <c r="H1" s="449"/>
+    </row>
+    <row r="2" spans="1:8" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="167" t="s">
         <v>157</v>
       </c>
@@ -8773,41 +8773,41 @@
         <v>159</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="443" t="s">
+    <row r="3" spans="1:8" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="445" t="s">
         <v>160</v>
       </c>
-      <c r="B3" s="444"/>
+      <c r="B3" s="446"/>
       <c r="C3" s="169"/>
       <c r="D3" s="194" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="443"/>
-      <c r="B4" s="445"/>
+    <row r="4" spans="1:8" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="445"/>
+      <c r="B4" s="447"/>
       <c r="C4" s="170"/>
       <c r="D4" s="195" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="443"/>
-      <c r="B5" s="445"/>
+    <row r="5" spans="1:8" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="445"/>
+      <c r="B5" s="447"/>
       <c r="C5" s="170"/>
       <c r="D5" s="196" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="443"/>
-      <c r="B6" s="446"/>
+    <row r="6" spans="1:8" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="445"/>
+      <c r="B6" s="448"/>
       <c r="C6" s="171"/>
       <c r="D6" s="197" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="182" t="s">
         <v>165</v>
       </c>
@@ -8836,27 +8836,27 @@
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.125" customWidth="1"/>
-    <col min="2" max="2" width="8.875" style="174"/>
-    <col min="3" max="3" width="11.125" style="174" bestFit="1" customWidth="1"/>
-    <col min="4" max="12" width="11.625" style="174" bestFit="1" customWidth="1"/>
-    <col min="13" max="15" width="12.625" style="174" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.09765625" customWidth="1"/>
+    <col min="2" max="2" width="8.8984375" style="174"/>
+    <col min="3" max="3" width="11.09765625" style="174" bestFit="1" customWidth="1"/>
+    <col min="4" max="12" width="11.59765625" style="174" bestFit="1" customWidth="1"/>
+    <col min="13" max="15" width="12.59765625" style="174" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" s="181"/>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="183" t="s">
         <v>167</v>
       </c>
       <c r="N2" s="192"/>
       <c r="O2" s="192"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="448"/>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A3" s="450"/>
       <c r="B3" s="175" t="s">
         <v>170</v>
       </c>
@@ -8878,8 +8878,8 @@
       <c r="N3"/>
       <c r="O3"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="448"/>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A4" s="450"/>
       <c r="B4" s="153" t="s">
         <v>171</v>
       </c>
@@ -8899,8 +8899,8 @@
       <c r="N4" s="192"/>
       <c r="O4" s="192"/>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="448"/>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A5" s="450"/>
       <c r="B5" s="153" t="s">
         <v>172</v>
       </c>
@@ -8920,8 +8920,8 @@
       <c r="N5" s="192"/>
       <c r="O5" s="192"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="448"/>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A6" s="450"/>
       <c r="B6" s="153" t="s">
         <v>173</v>
       </c>
@@ -8941,8 +8941,8 @@
       <c r="N6" s="192"/>
       <c r="O6" s="192"/>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="448"/>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A7" s="450"/>
       <c r="B7" s="153" t="s">
         <v>174</v>
       </c>
@@ -8962,10 +8962,10 @@
       <c r="N7" s="192"/>
       <c r="O7" s="192"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" s="154"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="F10" s="192"/>
       <c r="G10" s="192"/>
       <c r="H10" s="192"/>
@@ -8975,7 +8975,7 @@
       <c r="L10" s="192"/>
       <c r="M10" s="192"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" s="184" t="s">
         <v>168</v>
       </c>
@@ -8991,8 +8991,8 @@
       <c r="N11"/>
       <c r="O11"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="449"/>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A12" s="451"/>
       <c r="B12" s="175" t="s">
         <v>170</v>
       </c>
@@ -9014,8 +9014,8 @@
       <c r="N12"/>
       <c r="O12"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="449"/>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A13" s="451"/>
       <c r="B13" s="153" t="s">
         <v>171</v>
       </c>
@@ -9035,8 +9035,8 @@
       <c r="N13"/>
       <c r="O13"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="449"/>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A14" s="451"/>
       <c r="B14" s="153" t="s">
         <v>172</v>
       </c>
@@ -9056,8 +9056,8 @@
       <c r="N14"/>
       <c r="O14"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="449"/>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A15" s="451"/>
       <c r="B15" s="153" t="s">
         <v>173</v>
       </c>
@@ -9077,8 +9077,8 @@
       <c r="N15"/>
       <c r="O15"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="449"/>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A16" s="451"/>
       <c r="B16" s="153" t="s">
         <v>174</v>
       </c>
@@ -9098,7 +9098,7 @@
       <c r="N16"/>
       <c r="O16"/>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" s="154"/>
       <c r="D17" s="192"/>
       <c r="E17" s="192"/>
@@ -9113,7 +9113,7 @@
       <c r="N17"/>
       <c r="O17"/>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18" s="154"/>
       <c r="D18" s="192"/>
       <c r="E18" s="192"/>
@@ -9126,7 +9126,7 @@
       <c r="L18" s="192"/>
       <c r="M18" s="192"/>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19" s="154"/>
       <c r="D19" s="192"/>
       <c r="E19" s="192"/>
@@ -9139,7 +9139,7 @@
       <c r="L19" s="192"/>
       <c r="M19" s="192"/>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20" s="154"/>
       <c r="D20" s="192"/>
       <c r="E20" s="192"/>
@@ -9152,7 +9152,7 @@
       <c r="L20" s="192"/>
       <c r="M20" s="192"/>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21" s="154"/>
       <c r="D21" s="192"/>
       <c r="E21" s="192"/>
@@ -9165,7 +9165,7 @@
       <c r="L21" s="192"/>
       <c r="M21" s="192"/>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A22" s="154"/>
       <c r="D22" s="192"/>
       <c r="E22" s="192"/>
@@ -9178,7 +9178,7 @@
       <c r="L22" s="192"/>
       <c r="M22" s="192"/>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A23" s="154"/>
       <c r="D23" s="192"/>
       <c r="E23" s="192"/>
@@ -9191,7 +9191,7 @@
       <c r="L23" s="192"/>
       <c r="M23" s="192"/>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A24" s="154"/>
       <c r="D24" s="192"/>
       <c r="E24" s="192"/>
@@ -9204,7 +9204,7 @@
       <c r="L24" s="192"/>
       <c r="M24" s="192"/>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A25" s="154"/>
       <c r="D25" s="192"/>
       <c r="E25" s="192"/>
@@ -9217,7 +9217,7 @@
       <c r="L25" s="192"/>
       <c r="M25" s="192"/>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A26" s="154"/>
       <c r="D26" s="192"/>
       <c r="E26" s="192"/>
@@ -9230,7 +9230,7 @@
       <c r="L26" s="192"/>
       <c r="M26" s="192"/>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
       <c r="F28" s="192"/>
       <c r="G28" s="192"/>
       <c r="H28" s="192"/>
@@ -9240,7 +9240,7 @@
       <c r="N28"/>
       <c r="O28"/>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A29" s="192"/>
       <c r="B29" s="192"/>
       <c r="C29" s="192"/>
@@ -9255,7 +9255,7 @@
       <c r="N29"/>
       <c r="O29"/>
     </row>
-    <row r="30" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="192"/>
       <c r="B30" s="192"/>
       <c r="C30" s="192"/>
@@ -9270,7 +9270,7 @@
       <c r="N30"/>
       <c r="O30"/>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A31" s="192"/>
       <c r="B31" s="192"/>
       <c r="C31" s="192"/>
@@ -9285,7 +9285,7 @@
       <c r="N31"/>
       <c r="O31"/>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A32" s="192"/>
       <c r="B32" s="192"/>
       <c r="C32" s="192"/>
@@ -9300,7 +9300,7 @@
       <c r="N32"/>
       <c r="O32"/>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A33" s="192"/>
       <c r="B33" s="192"/>
       <c r="C33" s="192"/>
@@ -9315,7 +9315,7 @@
       <c r="N33"/>
       <c r="O33"/>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A34" s="192"/>
       <c r="B34" s="192"/>
       <c r="C34" s="192"/>
@@ -9330,7 +9330,7 @@
       <c r="N34"/>
       <c r="O34"/>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A35" s="154"/>
       <c r="D35" s="192"/>
       <c r="E35" s="192"/>
@@ -9343,7 +9343,7 @@
       <c r="N35"/>
       <c r="O35"/>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A36" s="154"/>
       <c r="D36" s="192"/>
       <c r="E36" s="192"/>
@@ -9356,7 +9356,7 @@
       <c r="N36"/>
       <c r="O36"/>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A37" s="154"/>
       <c r="D37" s="192"/>
       <c r="E37" s="192"/>
@@ -9365,7 +9365,7 @@
       <c r="H37" s="192"/>
       <c r="I37" s="192"/>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A38" s="154"/>
       <c r="D38" s="192"/>
       <c r="E38" s="192"/>
@@ -9374,22 +9374,22 @@
       <c r="H38" s="192"/>
       <c r="I38" s="192"/>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A39" s="154"/>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A40" s="154"/>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A41" s="154"/>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A42" s="154"/>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A43" s="154"/>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A44" s="154"/>
     </row>
   </sheetData>
@@ -9413,45 +9413,45 @@
       <selection pane="bottomRight" activeCell="T2" sqref="T2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.625" style="25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.375" style="76" customWidth="1"/>
+    <col min="1" max="1" width="16.59765625" style="25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.3984375" style="76" customWidth="1"/>
     <col min="3" max="3" width="14" style="4" customWidth="1"/>
-    <col min="4" max="4" width="20.125" style="25" customWidth="1"/>
-    <col min="5" max="5" width="52.625" style="27" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.375" style="4" customWidth="1"/>
+    <col min="4" max="4" width="20.09765625" style="25" customWidth="1"/>
+    <col min="5" max="5" width="52.59765625" style="27" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.3984375" style="4" customWidth="1"/>
     <col min="7" max="7" width="36.5" style="27" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="54.625" style="31" customWidth="1"/>
-    <col min="9" max="9" width="38.375" style="45" customWidth="1"/>
+    <col min="8" max="8" width="54.59765625" style="31" customWidth="1"/>
+    <col min="9" max="9" width="38.3984375" style="45" customWidth="1"/>
     <col min="10" max="10" width="36.5" style="45" customWidth="1"/>
-    <col min="11" max="12" width="17.125" style="31" customWidth="1"/>
-    <col min="13" max="13" width="25.875" style="27" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="49.625" style="4" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="43.625" style="49" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="32.875" style="49" customWidth="1"/>
-    <col min="17" max="17" width="10.75" style="69" customWidth="1"/>
-    <col min="18" max="18" width="17.25" style="69" customWidth="1"/>
-    <col min="19" max="19" width="15.625" style="69" customWidth="1"/>
-    <col min="20" max="20" width="17.125" style="69" customWidth="1"/>
+    <col min="11" max="12" width="17.09765625" style="31" customWidth="1"/>
+    <col min="13" max="13" width="25.8984375" style="27" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="49.59765625" style="4" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="43.59765625" style="49" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="32.8984375" style="49" customWidth="1"/>
+    <col min="17" max="17" width="10.69921875" style="69" customWidth="1"/>
+    <col min="18" max="18" width="17.19921875" style="69" customWidth="1"/>
+    <col min="19" max="19" width="15.59765625" style="69" customWidth="1"/>
+    <col min="20" max="20" width="17.09765625" style="69" customWidth="1"/>
     <col min="21" max="21" width="16.5" style="69" customWidth="1"/>
-    <col min="22" max="22" width="5.75" style="69" customWidth="1"/>
-    <col min="23" max="23" width="17.375" style="11" customWidth="1"/>
-    <col min="24" max="24" width="29.125" style="11" customWidth="1"/>
+    <col min="22" max="22" width="5.69921875" style="69" customWidth="1"/>
+    <col min="23" max="23" width="17.3984375" style="11" customWidth="1"/>
+    <col min="24" max="24" width="29.09765625" style="11" customWidth="1"/>
     <col min="25" max="25" width="15" style="11" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="11.5" style="11" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="15" style="11" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="13" style="11" customWidth="1"/>
     <col min="29" max="31" width="11.5" style="11" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="12.875" style="11" customWidth="1"/>
+    <col min="32" max="32" width="12.8984375" style="11" customWidth="1"/>
     <col min="33" max="35" width="15" style="11" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="11.5" style="40" customWidth="1"/>
-    <col min="37" max="39" width="12.125" style="4" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="10.125" style="4" bestFit="1" customWidth="1"/>
-    <col min="41" max="16384" width="8.625" style="4"/>
+    <col min="37" max="39" width="12.09765625" style="4" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="10.09765625" style="4" bestFit="1" customWidth="1"/>
+    <col min="41" max="16384" width="8.59765625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" ht="16.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:40" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B1" s="25"/>
       <c r="C1" s="25"/>
       <c r="E1" s="25"/>
@@ -9474,32 +9474,32 @@
       <c r="V1" s="25"/>
       <c r="W1" s="25"/>
       <c r="X1" s="25"/>
-      <c r="Y1" s="431" t="s">
+      <c r="Y1" s="433" t="s">
         <v>12</v>
       </c>
-      <c r="Z1" s="432"/>
-      <c r="AA1" s="432"/>
-      <c r="AB1" s="433"/>
-      <c r="AC1" s="431" t="s">
+      <c r="Z1" s="434"/>
+      <c r="AA1" s="434"/>
+      <c r="AB1" s="435"/>
+      <c r="AC1" s="433" t="s">
         <v>13</v>
       </c>
-      <c r="AD1" s="432"/>
-      <c r="AE1" s="432"/>
-      <c r="AF1" s="433"/>
-      <c r="AG1" s="434" t="s">
+      <c r="AD1" s="434"/>
+      <c r="AE1" s="434"/>
+      <c r="AF1" s="435"/>
+      <c r="AG1" s="436" t="s">
         <v>14</v>
       </c>
-      <c r="AH1" s="435"/>
-      <c r="AI1" s="435"/>
-      <c r="AJ1" s="435"/>
-      <c r="AK1" s="434" t="s">
+      <c r="AH1" s="437"/>
+      <c r="AI1" s="437"/>
+      <c r="AJ1" s="437"/>
+      <c r="AK1" s="436" t="s">
         <v>68</v>
       </c>
-      <c r="AL1" s="435"/>
-      <c r="AM1" s="435"/>
-      <c r="AN1" s="435"/>
-    </row>
-    <row r="2" spans="1:40" s="275" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="AL1" s="437"/>
+      <c r="AM1" s="437"/>
+      <c r="AN1" s="437"/>
+    </row>
+    <row r="2" spans="1:40" s="275" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A2" s="44" t="s">
         <v>71</v>
       </c>
@@ -9621,7 +9621,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="3" spans="1:40" ht="51" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:40" ht="69" x14ac:dyDescent="0.3">
       <c r="A3" s="394" t="s">
         <v>72</v>
       </c>
@@ -9704,7 +9704,7 @@
       <c r="AM3" s="20"/>
       <c r="AN3" s="20"/>
     </row>
-    <row r="4" spans="1:40" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:40" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A4" s="358" t="s">
         <v>72</v>
       </c>
@@ -9788,7 +9788,7 @@
       <c r="AM4" s="20"/>
       <c r="AN4" s="20"/>
     </row>
-    <row r="5" spans="1:40" ht="178.5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:40" ht="193.2" x14ac:dyDescent="0.3">
       <c r="A5" s="390" t="s">
         <v>72</v>
       </c>
@@ -9890,7 +9890,7 @@
       <c r="AM5" s="20"/>
       <c r="AN5" s="20"/>
     </row>
-    <row r="6" spans="1:40" ht="204" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:40" ht="220.8" x14ac:dyDescent="0.3">
       <c r="A6" s="390" t="s">
         <v>72</v>
       </c>
@@ -9992,7 +9992,7 @@
       <c r="AM6" s="20"/>
       <c r="AN6" s="20"/>
     </row>
-    <row r="7" spans="1:40" ht="255" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:40" ht="276" x14ac:dyDescent="0.3">
       <c r="A7" s="390" t="s">
         <v>72</v>
       </c>
@@ -10094,7 +10094,7 @@
       <c r="AM7" s="20"/>
       <c r="AN7" s="20"/>
     </row>
-    <row r="8" spans="1:40" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:40" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A8" s="358" t="s">
         <v>72</v>
       </c>
@@ -10178,7 +10178,7 @@
       <c r="AM8" s="20"/>
       <c r="AN8" s="20"/>
     </row>
-    <row r="9" spans="1:40" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:40" ht="69" x14ac:dyDescent="0.3">
       <c r="A9" s="358" t="s">
         <v>72</v>
       </c>
@@ -10263,7 +10263,7 @@
       <c r="AM9" s="20"/>
       <c r="AN9" s="20"/>
     </row>
-    <row r="10" spans="1:40" ht="51" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:40" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A10" s="394" t="s">
         <v>72</v>
       </c>
@@ -10345,7 +10345,7 @@
       <c r="AM10" s="20"/>
       <c r="AN10" s="20"/>
     </row>
-    <row r="11" spans="1:40" ht="51" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:40" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A11" s="358" t="s">
         <v>72</v>
       </c>
@@ -10429,7 +10429,7 @@
       <c r="AM11" s="278"/>
       <c r="AN11" s="278"/>
     </row>
-    <row r="12" spans="1:40" ht="51" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:40" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A12" s="358" t="s">
         <v>72</v>
       </c>
@@ -10514,7 +10514,7 @@
       <c r="AM12" s="278"/>
       <c r="AN12" s="278"/>
     </row>
-    <row r="13" spans="1:40" ht="127.5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:40" ht="138" x14ac:dyDescent="0.3">
       <c r="A13" s="358" t="s">
         <v>72</v>
       </c>
@@ -10627,7 +10627,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:40" ht="51" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:40" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A14" s="358" t="s">
         <v>72</v>
       </c>
@@ -10708,7 +10708,7 @@
       <c r="AM14" s="278"/>
       <c r="AN14" s="278"/>
     </row>
-    <row r="15" spans="1:40" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:40" ht="96.6" x14ac:dyDescent="0.3">
       <c r="A15" s="371" t="s">
         <v>72</v>
       </c>
@@ -10788,7 +10788,7 @@
       <c r="AM15" s="278"/>
       <c r="AN15" s="278"/>
     </row>
-    <row r="16" spans="1:40" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:40" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A16" s="358" t="s">
         <v>72</v>
       </c>
@@ -10871,7 +10871,7 @@
       <c r="AM16" s="20"/>
       <c r="AN16" s="20"/>
     </row>
-    <row r="17" spans="1:40" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:40" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A17" s="358" t="s">
         <v>72</v>
       </c>
@@ -10953,7 +10953,7 @@
       <c r="AM17" s="20"/>
       <c r="AN17" s="20"/>
     </row>
-    <row r="18" spans="1:40" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:40" ht="69" x14ac:dyDescent="0.3">
       <c r="A18" s="358" t="s">
         <v>72</v>
       </c>
@@ -11036,7 +11036,7 @@
       <c r="AM18" s="20"/>
       <c r="AN18" s="20"/>
     </row>
-    <row r="19" spans="1:40" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:40" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A19" s="374" t="s">
         <v>72</v>
       </c>
@@ -11118,7 +11118,7 @@
       <c r="AM19" s="20"/>
       <c r="AN19" s="20"/>
     </row>
-    <row r="20" spans="1:40" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:40" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A20" s="374" t="s">
         <v>72</v>
       </c>
@@ -11200,7 +11200,7 @@
       <c r="AM20" s="20"/>
       <c r="AN20" s="20"/>
     </row>
-    <row r="21" spans="1:40" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:40" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A21" s="394" t="s">
         <v>72</v>
       </c>
@@ -11280,7 +11280,7 @@
       <c r="AM21" s="20"/>
       <c r="AN21" s="20"/>
     </row>
-    <row r="22" spans="1:40" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:40" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A22" s="358" t="s">
         <v>72</v>
       </c>
@@ -11362,7 +11362,7 @@
       <c r="AM22" s="20"/>
       <c r="AN22" s="20"/>
     </row>
-    <row r="23" spans="1:40" ht="51" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:40" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A23" s="392" t="s">
         <v>72</v>
       </c>
@@ -11441,7 +11441,7 @@
       <c r="AM23" s="20"/>
       <c r="AN23" s="20"/>
     </row>
-    <row r="24" spans="1:40" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:40" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A24" s="358" t="s">
         <v>72</v>
       </c>
@@ -11523,7 +11523,7 @@
       <c r="AM24" s="20"/>
       <c r="AN24" s="20"/>
     </row>
-    <row r="25" spans="1:40" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:40" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A25" s="358" t="s">
         <v>72</v>
       </c>
@@ -11605,7 +11605,7 @@
       <c r="AM25" s="20"/>
       <c r="AN25" s="20"/>
     </row>
-    <row r="26" spans="1:40" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:40" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A26" s="358" t="s">
         <v>72</v>
       </c>
@@ -11687,7 +11687,7 @@
       <c r="AM26" s="20"/>
       <c r="AN26" s="20"/>
     </row>
-    <row r="27" spans="1:40" ht="51" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:40" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A27" s="358" t="s">
         <v>72</v>
       </c>
@@ -11769,7 +11769,7 @@
       <c r="AM27" s="20"/>
       <c r="AN27" s="20"/>
     </row>
-    <row r="28" spans="1:40" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:40" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A28" s="394" t="s">
         <v>72</v>
       </c>
@@ -11849,7 +11849,7 @@
       <c r="AM28" s="20"/>
       <c r="AN28" s="20"/>
     </row>
-    <row r="29" spans="1:40" s="286" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:40" s="286" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A29" s="374" t="s">
         <v>72</v>
       </c>
@@ -11928,7 +11928,7 @@
       <c r="AM29" s="234"/>
       <c r="AN29" s="234"/>
     </row>
-    <row r="30" spans="1:40" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:40" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A30" s="358" t="s">
         <v>72</v>
       </c>
@@ -12010,7 +12010,7 @@
       <c r="AM30" s="20"/>
       <c r="AN30" s="20"/>
     </row>
-    <row r="31" spans="1:40" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:40" ht="69" x14ac:dyDescent="0.3">
       <c r="A31" s="358" t="s">
         <v>72</v>
       </c>
@@ -12093,7 +12093,7 @@
       <c r="AM31" s="20"/>
       <c r="AN31" s="20"/>
     </row>
-    <row r="32" spans="1:40" s="286" customFormat="1" ht="153" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:40" s="286" customFormat="1" ht="151.80000000000001" x14ac:dyDescent="0.3">
       <c r="A32" s="394" t="s">
         <v>72</v>
       </c>
@@ -12252,66 +12252,66 @@
       <selection pane="bottomRight" activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.625" style="25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.59765625" style="25" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="52.5" style="76" customWidth="1"/>
     <col min="3" max="3" width="6.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.625" style="25" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.625" style="27" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.875" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="55.125" style="27" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="78.75" style="50" customWidth="1"/>
-    <col min="9" max="9" width="57.625" style="62" customWidth="1"/>
+    <col min="4" max="4" width="29.59765625" style="25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.59765625" style="27" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.8984375" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="55.09765625" style="27" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="78.69921875" style="50" customWidth="1"/>
+    <col min="9" max="9" width="57.59765625" style="62" customWidth="1"/>
     <col min="10" max="10" width="28" style="45" customWidth="1"/>
-    <col min="11" max="12" width="17.125" style="31" customWidth="1"/>
-    <col min="13" max="13" width="26.375" style="27" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="56.625" style="4" customWidth="1"/>
-    <col min="15" max="15" width="34.625" style="49" customWidth="1"/>
-    <col min="16" max="16" width="41.875" style="49" customWidth="1"/>
-    <col min="17" max="18" width="13.125" style="69" customWidth="1"/>
-    <col min="19" max="19" width="14.875" style="69" customWidth="1"/>
-    <col min="20" max="20" width="15.625" style="69" customWidth="1"/>
+    <col min="11" max="12" width="17.09765625" style="31" customWidth="1"/>
+    <col min="13" max="13" width="26.3984375" style="27" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="56.59765625" style="4" customWidth="1"/>
+    <col min="15" max="15" width="34.59765625" style="49" customWidth="1"/>
+    <col min="16" max="16" width="41.8984375" style="49" customWidth="1"/>
+    <col min="17" max="18" width="13.09765625" style="69" customWidth="1"/>
+    <col min="19" max="19" width="14.8984375" style="69" customWidth="1"/>
+    <col min="20" max="20" width="15.59765625" style="69" customWidth="1"/>
     <col min="21" max="21" width="22" style="69" customWidth="1"/>
-    <col min="22" max="22" width="18.875" style="69" customWidth="1"/>
-    <col min="23" max="23" width="7.75" style="69" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="18.8984375" style="69" customWidth="1"/>
+    <col min="23" max="23" width="7.69921875" style="69" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="7" style="69" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="20" style="11" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="68.75" style="11" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="12.25" style="11" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="68.69921875" style="11" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="12.19921875" style="11" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="11" style="4" customWidth="1"/>
-    <col min="29" max="31" width="8.625" style="4"/>
-    <col min="32" max="32" width="13.375" style="4" customWidth="1"/>
-    <col min="33" max="36" width="8.625" style="4"/>
-    <col min="37" max="37" width="15.875" style="11" customWidth="1"/>
-    <col min="38" max="38" width="18.25" style="11" customWidth="1"/>
-    <col min="39" max="39" width="14.625" style="11" customWidth="1"/>
-    <col min="40" max="40" width="17.375" style="11" customWidth="1"/>
-    <col min="41" max="41" width="50.625" style="4" bestFit="1" customWidth="1"/>
-    <col min="42" max="16384" width="8.625" style="4"/>
+    <col min="29" max="31" width="8.59765625" style="4"/>
+    <col min="32" max="32" width="13.3984375" style="4" customWidth="1"/>
+    <col min="33" max="36" width="8.59765625" style="4"/>
+    <col min="37" max="37" width="15.8984375" style="11" customWidth="1"/>
+    <col min="38" max="38" width="18.19921875" style="11" customWidth="1"/>
+    <col min="39" max="39" width="14.59765625" style="11" customWidth="1"/>
+    <col min="40" max="40" width="17.3984375" style="11" customWidth="1"/>
+    <col min="41" max="41" width="50.59765625" style="4" bestFit="1" customWidth="1"/>
+    <col min="42" max="16384" width="8.59765625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:41" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B1" s="4"/>
       <c r="O1" s="27"/>
       <c r="P1" s="27"/>
       <c r="Y1" s="70"/>
       <c r="Z1" s="70"/>
-      <c r="AB1" s="436" t="s">
+      <c r="AB1" s="438" t="s">
         <v>12</v>
       </c>
-      <c r="AC1" s="436"/>
-      <c r="AD1" s="436"/>
-      <c r="AE1" s="436" t="s">
+      <c r="AC1" s="438"/>
+      <c r="AD1" s="438"/>
+      <c r="AE1" s="438" t="s">
         <v>13</v>
       </c>
-      <c r="AF1" s="436"/>
-      <c r="AG1" s="436"/>
-      <c r="AH1" s="436" t="s">
+      <c r="AF1" s="438"/>
+      <c r="AG1" s="438"/>
+      <c r="AH1" s="438" t="s">
         <v>14</v>
       </c>
-      <c r="AI1" s="436"/>
-      <c r="AJ1" s="436"/>
+      <c r="AI1" s="438"/>
+      <c r="AJ1" s="438"/>
       <c r="AK1" s="105" t="s">
         <v>136</v>
       </c>
@@ -12325,7 +12325,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="2" spans="1:41" s="275" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:41" s="275" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A2" s="44" t="s">
         <v>71</v>
       </c>
@@ -12448,7 +12448,7 @@
       </c>
       <c r="AO2" s="4"/>
     </row>
-    <row r="3" spans="1:41" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:41" s="2" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A3" s="239" t="s">
         <v>35</v>
       </c>
@@ -12481,7 +12481,7 @@
         <v>28</v>
       </c>
       <c r="K3" s="198" t="s">
-        <v>1050</v>
+        <v>1048</v>
       </c>
       <c r="L3" s="47" t="s">
         <v>324</v>
@@ -12551,7 +12551,7 @@
       <c r="AM3" s="293"/>
       <c r="AN3" s="294"/>
     </row>
-    <row r="4" spans="1:41" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:41" s="2" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A4" s="239" t="s">
         <v>35</v>
       </c>
@@ -12585,7 +12585,7 @@
         <v>28</v>
       </c>
       <c r="K4" s="198" t="s">
-        <v>1050</v>
+        <v>1048</v>
       </c>
       <c r="L4" s="47" t="s">
         <v>324</v>
@@ -12655,7 +12655,7 @@
       <c r="AM4" s="293"/>
       <c r="AN4" s="294"/>
     </row>
-    <row r="5" spans="1:41" s="2" customFormat="1" ht="204" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:41" s="2" customFormat="1" ht="220.8" x14ac:dyDescent="0.3">
       <c r="A5" s="260" t="s">
         <v>35</v>
       </c>
@@ -12758,7 +12758,7 @@
       <c r="AM5" s="293"/>
       <c r="AN5" s="294"/>
     </row>
-    <row r="6" spans="1:41" s="2" customFormat="1" ht="102" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:41" s="2" customFormat="1" ht="110.4" x14ac:dyDescent="0.3">
       <c r="A6" s="260" t="s">
         <v>35</v>
       </c>
@@ -12844,7 +12844,7 @@
       <c r="AM6" s="293"/>
       <c r="AN6" s="294"/>
     </row>
-    <row r="7" spans="1:41" ht="127.5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:41" ht="138" x14ac:dyDescent="0.3">
       <c r="A7" s="296" t="s">
         <v>34</v>
       </c>
@@ -12923,7 +12923,7 @@
       <c r="AM7" s="298"/>
       <c r="AN7" s="299"/>
     </row>
-    <row r="8" spans="1:41" s="2" customFormat="1" ht="90.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:41" s="2" customFormat="1" ht="90.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="257" t="s">
         <v>34</v>
       </c>
@@ -12956,7 +12956,7 @@
         <v>27</v>
       </c>
       <c r="K8" s="198" t="s">
-        <v>1050</v>
+        <v>1048</v>
       </c>
       <c r="L8" s="47" t="s">
         <v>106</v>
@@ -13034,7 +13034,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:41" s="2" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:41" s="2" customFormat="1" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A9" s="301" t="s">
         <v>34</v>
       </c>
@@ -13067,7 +13067,7 @@
         <v>507</v>
       </c>
       <c r="K9" s="198" t="s">
-        <v>1050</v>
+        <v>1048</v>
       </c>
       <c r="L9" s="47" t="s">
         <v>106</v>
@@ -13145,7 +13145,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:41" s="2" customFormat="1" ht="87" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:41" s="2" customFormat="1" ht="87" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="240" t="s">
         <v>34</v>
       </c>
@@ -13179,7 +13179,7 @@
         <v>27</v>
       </c>
       <c r="K10" s="198" t="s">
-        <v>1050</v>
+        <v>1048</v>
       </c>
       <c r="L10" s="47" t="s">
         <v>106</v>
@@ -13247,7 +13247,7 @@
       <c r="AM10" s="74"/>
       <c r="AN10" s="74"/>
     </row>
-    <row r="11" spans="1:41" s="2" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:41" s="2" customFormat="1" ht="82.8" x14ac:dyDescent="0.3">
       <c r="A11" s="240" t="s">
         <v>34</v>
       </c>
@@ -13281,7 +13281,7 @@
         <v>27</v>
       </c>
       <c r="K11" s="198" t="s">
-        <v>1050</v>
+        <v>1048</v>
       </c>
       <c r="L11" s="47" t="s">
         <v>106</v>
@@ -13349,7 +13349,7 @@
       <c r="AM11" s="74"/>
       <c r="AN11" s="74"/>
     </row>
-    <row r="12" spans="1:41" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:41" ht="69" x14ac:dyDescent="0.3">
       <c r="A12" s="296" t="s">
         <v>179</v>
       </c>
@@ -13390,7 +13390,7 @@
         <v>376</v>
       </c>
       <c r="O12" s="55" t="s">
-        <v>1052</v>
+        <v>1050</v>
       </c>
       <c r="P12" s="55" t="s">
         <v>797</v>
@@ -13428,7 +13428,7 @@
       <c r="AM12" s="298"/>
       <c r="AN12" s="299"/>
     </row>
-    <row r="13" spans="1:41" s="2" customFormat="1" ht="191.25" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:41" s="2" customFormat="1" ht="207" x14ac:dyDescent="0.3">
       <c r="A13" s="260" t="s">
         <v>179</v>
       </c>
@@ -13462,7 +13462,7 @@
         <v>28</v>
       </c>
       <c r="K13" s="198" t="s">
-        <v>1050</v>
+        <v>1048</v>
       </c>
       <c r="L13" s="47" t="s">
         <v>106</v>
@@ -13472,7 +13472,7 @@
       </c>
       <c r="N13" s="100"/>
       <c r="O13" s="79" t="s">
-        <v>1051</v>
+        <v>1049</v>
       </c>
       <c r="P13" s="79" t="s">
         <v>481</v>
@@ -13529,7 +13529,7 @@
       <c r="AN13" s="294"/>
       <c r="AO13" s="208"/>
     </row>
-    <row r="14" spans="1:41" s="306" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:41" s="306" customFormat="1" ht="82.8" x14ac:dyDescent="0.3">
       <c r="A14" s="305" t="s">
         <v>179</v>
       </c>
@@ -13562,7 +13562,7 @@
         <v>28</v>
       </c>
       <c r="K14" s="198" t="s">
-        <v>1050</v>
+        <v>1048</v>
       </c>
       <c r="L14" s="47" t="s">
         <v>106</v>
@@ -13612,7 +13612,7 @@
       <c r="AM14" s="281"/>
       <c r="AN14" s="307"/>
     </row>
-    <row r="15" spans="1:41" ht="51" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:41" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A15" s="296" t="s">
         <v>180</v>
       </c>
@@ -13691,7 +13691,7 @@
       <c r="AM15" s="298"/>
       <c r="AN15" s="299"/>
     </row>
-    <row r="16" spans="1:41" s="2" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:41" s="2" customFormat="1" ht="82.8" x14ac:dyDescent="0.3">
       <c r="A16" s="296" t="s">
         <v>180</v>
       </c>
@@ -13724,7 +13724,7 @@
         <v>183</v>
       </c>
       <c r="K16" s="198" t="s">
-        <v>1050</v>
+        <v>1048</v>
       </c>
       <c r="L16" s="47" t="s">
         <v>106</v>
@@ -13790,7 +13790,7 @@
       <c r="AM16" s="57"/>
       <c r="AN16" s="281"/>
     </row>
-    <row r="17" spans="1:40" ht="102" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:40" ht="110.4" x14ac:dyDescent="0.3">
       <c r="A17" s="309" t="s">
         <v>698</v>
       </c>
@@ -13869,7 +13869,7 @@
       <c r="AM17" s="298"/>
       <c r="AN17" s="299"/>
     </row>
-    <row r="18" spans="1:40" s="2" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:40" s="2" customFormat="1" ht="82.8" x14ac:dyDescent="0.3">
       <c r="A18" s="310" t="s">
         <v>698</v>
       </c>
@@ -13903,7 +13903,7 @@
         <v>491</v>
       </c>
       <c r="K18" s="198" t="s">
-        <v>1050</v>
+        <v>1048</v>
       </c>
       <c r="L18" s="47" t="s">
         <v>106</v>
@@ -13981,7 +13981,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:40" s="2" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:40" s="2" customFormat="1" ht="82.8" x14ac:dyDescent="0.3">
       <c r="A19" s="310" t="s">
         <v>698</v>
       </c>
@@ -14015,7 +14015,7 @@
         <v>491</v>
       </c>
       <c r="K19" s="198" t="s">
-        <v>1050</v>
+        <v>1048</v>
       </c>
       <c r="L19" s="47" t="s">
         <v>106</v>
@@ -14093,7 +14093,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:40" s="2" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:40" s="2" customFormat="1" ht="82.8" x14ac:dyDescent="0.3">
       <c r="A20" s="301" t="s">
         <v>698</v>
       </c>
@@ -14127,7 +14127,7 @@
         <v>491</v>
       </c>
       <c r="K20" s="198" t="s">
-        <v>1050</v>
+        <v>1048</v>
       </c>
       <c r="L20" s="47" t="s">
         <v>106</v>
@@ -14142,7 +14142,7 @@
         <v>514</v>
       </c>
       <c r="P20" s="77" t="s">
-        <v>1004</v>
+        <v>1002</v>
       </c>
       <c r="Q20" s="6">
         <v>2</v>
@@ -14205,7 +14205,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:40" s="2" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:40" s="2" customFormat="1" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A21" s="301" t="s">
         <v>698</v>
       </c>
@@ -14239,7 +14239,7 @@
         <v>507</v>
       </c>
       <c r="K21" s="198" t="s">
-        <v>1050</v>
+        <v>1048</v>
       </c>
       <c r="L21" s="47" t="s">
         <v>106</v>
@@ -14317,7 +14317,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:40" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:40" s="2" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A22" s="314" t="s">
         <v>519</v>
       </c>
@@ -14350,7 +14350,7 @@
         <v>523</v>
       </c>
       <c r="K22" s="198" t="s">
-        <v>1050</v>
+        <v>1048</v>
       </c>
       <c r="L22" s="47" t="s">
         <v>106</v>
@@ -14428,7 +14428,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:40" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:40" s="2" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A23" s="314" t="s">
         <v>519</v>
       </c>
@@ -14542,7 +14542,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:40" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:40" s="2" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A24" s="314" t="s">
         <v>531</v>
       </c>
@@ -14576,7 +14576,7 @@
         <v>523</v>
       </c>
       <c r="K24" s="198" t="s">
-        <v>1050</v>
+        <v>1048</v>
       </c>
       <c r="L24" s="47" t="s">
         <v>106</v>
@@ -14654,7 +14654,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:40" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:40" s="2" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A25" s="314" t="s">
         <v>531</v>
       </c>
@@ -14768,7 +14768,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="1:40" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:40" s="2" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A26" s="314" t="s">
         <v>531</v>
       </c>
@@ -14802,7 +14802,7 @@
         <v>523</v>
       </c>
       <c r="K26" s="198" t="s">
-        <v>1050</v>
+        <v>1048</v>
       </c>
       <c r="L26" s="47" t="s">
         <v>106</v>
@@ -14880,7 +14880,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:40" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:40" s="2" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A27" s="314" t="s">
         <v>531</v>
       </c>
@@ -14994,7 +14994,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="1:40" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:40" s="2" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A28" s="314" t="s">
         <v>355</v>
       </c>
@@ -15028,7 +15028,7 @@
         <v>549</v>
       </c>
       <c r="K28" s="198" t="s">
-        <v>1050</v>
+        <v>1048</v>
       </c>
       <c r="L28" s="47" t="s">
         <v>106</v>
@@ -15106,7 +15106,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:40" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:40" s="2" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A29" s="314" t="s">
         <v>551</v>
       </c>
@@ -15140,7 +15140,7 @@
         <v>523</v>
       </c>
       <c r="K29" s="198" t="s">
-        <v>1050</v>
+        <v>1048</v>
       </c>
       <c r="L29" s="47" t="s">
         <v>106</v>
@@ -15218,7 +15218,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:40" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:40" s="2" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A30" s="314" t="s">
         <v>551</v>
       </c>
@@ -15332,7 +15332,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:40" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:40" s="2" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A31" s="314" t="s">
         <v>557</v>
       </c>
@@ -15366,7 +15366,7 @@
         <v>561</v>
       </c>
       <c r="K31" s="198" t="s">
-        <v>1050</v>
+        <v>1048</v>
       </c>
       <c r="L31" s="47" t="s">
         <v>106</v>
@@ -15607,81 +15607,81 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AN15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="70" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="70" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="P9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight" activeCell="R16" sqref="R16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.25" style="319" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="73.625" style="272" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.875" style="269" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="55.25" style="319" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.75" style="320" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.125" style="269" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.25" style="320" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="175.625" style="321" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.19921875" style="319" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="73.59765625" style="272" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.8984375" style="269" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="55.19921875" style="319" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.69921875" style="320" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.09765625" style="269" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.19921875" style="320" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="175.59765625" style="321" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="17" style="322" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="19" style="322" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.625" style="321" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.59765625" style="321" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="26.5" style="321" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.75" style="320" customWidth="1"/>
-    <col min="14" max="14" width="31.75" style="269" customWidth="1"/>
-    <col min="15" max="16" width="28.25" style="355" customWidth="1"/>
+    <col min="13" max="13" width="15.69921875" style="320" customWidth="1"/>
+    <col min="14" max="14" width="31.69921875" style="269" customWidth="1"/>
+    <col min="15" max="16" width="28.19921875" style="355" customWidth="1"/>
     <col min="17" max="17" width="13" style="323" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="21.625" style="323" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="20.875" style="323" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="28.625" style="323" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.375" style="323" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="12.375" style="323" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="30.125" style="356" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="18.75" style="356" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="21.59765625" style="323" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="20.8984375" style="323" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="28.59765625" style="323" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.3984375" style="323" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.3984375" style="323" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="30.09765625" style="356" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="18.69921875" style="356" bestFit="1" customWidth="1"/>
     <col min="25" max="27" width="12.5" style="356" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="15.5" style="356" bestFit="1" customWidth="1"/>
     <col min="29" max="31" width="12.5" style="356" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="15.5" style="356" bestFit="1" customWidth="1"/>
     <col min="33" max="35" width="12.5" style="356" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="15.875" style="357" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="15.8984375" style="357" bestFit="1" customWidth="1"/>
     <col min="37" max="39" width="12.5" style="269" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="15.875" style="269" bestFit="1" customWidth="1"/>
-    <col min="41" max="16384" width="8.625" style="269"/>
+    <col min="40" max="40" width="15.8984375" style="269" bestFit="1" customWidth="1"/>
+    <col min="41" max="16384" width="8.59765625" style="269"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:40" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B1" s="269"/>
       <c r="O1" s="320"/>
       <c r="P1" s="320"/>
       <c r="W1" s="324"/>
       <c r="X1" s="324"/>
-      <c r="Y1" s="437" t="s">
+      <c r="Y1" s="439" t="s">
         <v>12</v>
       </c>
-      <c r="Z1" s="438"/>
-      <c r="AA1" s="438"/>
-      <c r="AB1" s="439"/>
-      <c r="AC1" s="437" t="s">
+      <c r="Z1" s="440"/>
+      <c r="AA1" s="440"/>
+      <c r="AB1" s="441"/>
+      <c r="AC1" s="439" t="s">
         <v>13</v>
       </c>
-      <c r="AD1" s="438"/>
-      <c r="AE1" s="438"/>
-      <c r="AF1" s="439"/>
-      <c r="AG1" s="440" t="s">
+      <c r="AD1" s="440"/>
+      <c r="AE1" s="440"/>
+      <c r="AF1" s="441"/>
+      <c r="AG1" s="442" t="s">
         <v>14</v>
       </c>
-      <c r="AH1" s="441"/>
-      <c r="AI1" s="441"/>
-      <c r="AJ1" s="441"/>
-      <c r="AK1" s="440" t="s">
+      <c r="AH1" s="443"/>
+      <c r="AI1" s="443"/>
+      <c r="AJ1" s="443"/>
+      <c r="AK1" s="442" t="s">
         <v>68</v>
       </c>
-      <c r="AL1" s="441"/>
-      <c r="AM1" s="441"/>
-      <c r="AN1" s="441"/>
-    </row>
-    <row r="2" spans="1:40" s="340" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="AL1" s="443"/>
+      <c r="AM1" s="443"/>
+      <c r="AN1" s="443"/>
+    </row>
+    <row r="2" spans="1:40" s="340" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="325" t="s">
         <v>71</v>
       </c>
@@ -15803,7 +15803,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="3" spans="1:40" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:40" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="268" t="s">
         <v>256</v>
       </c>
@@ -15886,7 +15886,7 @@
       <c r="AM3" s="353"/>
       <c r="AN3" s="353"/>
     </row>
-    <row r="4" spans="1:40" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:40" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="268" t="s">
         <v>259</v>
       </c>
@@ -15969,7 +15969,7 @@
       <c r="AM4" s="353"/>
       <c r="AN4" s="353"/>
     </row>
-    <row r="5" spans="1:40" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:40" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="268" t="s">
         <v>259</v>
       </c>
@@ -16053,7 +16053,7 @@
       <c r="AM5" s="353"/>
       <c r="AN5" s="353"/>
     </row>
-    <row r="6" spans="1:40" ht="60" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:40" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6" s="268" t="s">
         <v>259</v>
       </c>
@@ -16137,7 +16137,7 @@
       <c r="AM6" s="353"/>
       <c r="AN6" s="353"/>
     </row>
-    <row r="7" spans="1:40" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:40" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="425" t="s">
         <v>259</v>
       </c>
@@ -16221,7 +16221,7 @@
       <c r="AM7" s="353"/>
       <c r="AN7" s="353"/>
     </row>
-    <row r="8" spans="1:40" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:40" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="268" t="s">
         <v>263</v>
       </c>
@@ -16266,7 +16266,7 @@
         <v>669</v>
       </c>
       <c r="P8" s="423" t="s">
-        <v>1019</v>
+        <v>1017</v>
       </c>
       <c r="Q8" s="7">
         <v>1</v>
@@ -16305,7 +16305,7 @@
       <c r="AM8" s="353"/>
       <c r="AN8" s="353"/>
     </row>
-    <row r="9" spans="1:40" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:40" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="268" t="s">
         <v>263</v>
       </c>
@@ -16350,7 +16350,7 @@
         <v>671</v>
       </c>
       <c r="P9" s="423" t="s">
-        <v>1020</v>
+        <v>1018</v>
       </c>
       <c r="Q9" s="7">
         <v>1</v>
@@ -16389,7 +16389,7 @@
       <c r="AM9" s="353"/>
       <c r="AN9" s="353"/>
     </row>
-    <row r="10" spans="1:40" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:40" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="268" t="s">
         <v>263</v>
       </c>
@@ -16434,7 +16434,7 @@
         <v>380</v>
       </c>
       <c r="P10" s="423" t="s">
-        <v>1021</v>
+        <v>1019</v>
       </c>
       <c r="Q10" s="7">
         <v>1</v>
@@ -16473,7 +16473,7 @@
       <c r="AM10" s="353"/>
       <c r="AN10" s="353"/>
     </row>
-    <row r="11" spans="1:40" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:40" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="268" t="s">
         <v>266</v>
       </c>
@@ -16556,7 +16556,7 @@
       <c r="AM11" s="353"/>
       <c r="AN11" s="353"/>
     </row>
-    <row r="12" spans="1:40" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:40" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="268" t="s">
         <v>266</v>
       </c>
@@ -16639,7 +16639,7 @@
       <c r="AM12" s="353"/>
       <c r="AN12" s="353"/>
     </row>
-    <row r="13" spans="1:40" ht="60" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:40" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A13" s="268" t="s">
         <v>267</v>
       </c>
@@ -16722,7 +16722,7 @@
       <c r="AM13" s="353"/>
       <c r="AN13" s="353"/>
     </row>
-    <row r="14" spans="1:40" ht="60" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:40" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A14" s="268" t="s">
         <v>267</v>
       </c>
@@ -16805,7 +16805,7 @@
       <c r="AM14" s="353"/>
       <c r="AN14" s="353"/>
     </row>
-    <row r="15" spans="1:40" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:40" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="426" t="s">
         <v>263</v>
       </c>
@@ -16829,7 +16829,7 @@
         <v>103</v>
       </c>
       <c r="H15" s="384" t="s">
-        <v>1057</v>
+        <v>1055</v>
       </c>
       <c r="I15" s="344"/>
       <c r="J15" s="344"/>
@@ -16846,10 +16846,10 @@
         <v>361</v>
       </c>
       <c r="O15" s="423" t="s">
-        <v>1054</v>
-      </c>
-      <c r="P15" s="450" t="s">
-        <v>1053</v>
+        <v>1052</v>
+      </c>
+      <c r="P15" s="428" t="s">
+        <v>1051</v>
       </c>
       <c r="Q15" s="7">
         <v>1</v>
@@ -16864,7 +16864,7 @@
       <c r="W15" s="349" t="s">
         <v>4</v>
       </c>
-      <c r="X15" s="451" t="s">
+      <c r="X15" s="429" t="s">
         <v>473</v>
       </c>
       <c r="Y15" s="351"/>
@@ -16981,41 +16981,41 @@
       <selection pane="bottomRight" activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.75" style="18" customWidth="1"/>
+    <col min="1" max="1" width="22.69921875" style="18" customWidth="1"/>
     <col min="2" max="2" width="56" style="76" customWidth="1"/>
-    <col min="3" max="3" width="5.875" style="4" customWidth="1"/>
-    <col min="4" max="4" width="26.375" style="103" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.625" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.75" style="30" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="45.75" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="57.875" style="4" customWidth="1"/>
-    <col min="9" max="10" width="30.875" style="4" customWidth="1"/>
-    <col min="11" max="11" width="14.875" style="4" customWidth="1"/>
-    <col min="12" max="12" width="11.625" style="4" customWidth="1"/>
-    <col min="13" max="13" width="22.75" style="4" customWidth="1"/>
-    <col min="14" max="14" width="18.875" style="17" customWidth="1"/>
-    <col min="15" max="15" width="35.125" style="18" customWidth="1"/>
+    <col min="3" max="3" width="5.8984375" style="4" customWidth="1"/>
+    <col min="4" max="4" width="26.3984375" style="103" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.59765625" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.69921875" style="30" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="45.69921875" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="57.8984375" style="4" customWidth="1"/>
+    <col min="9" max="10" width="30.8984375" style="4" customWidth="1"/>
+    <col min="11" max="11" width="14.8984375" style="4" customWidth="1"/>
+    <col min="12" max="12" width="11.59765625" style="4" customWidth="1"/>
+    <col min="13" max="13" width="22.69921875" style="4" customWidth="1"/>
+    <col min="14" max="14" width="18.8984375" style="17" customWidth="1"/>
+    <col min="15" max="15" width="35.09765625" style="18" customWidth="1"/>
     <col min="16" max="16" width="36" style="18" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="13" style="4" customWidth="1"/>
-    <col min="18" max="18" width="15.375" style="4" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="19.625" style="4" bestFit="1" customWidth="1"/>
-    <col min="20" max="21" width="19.625" style="4" customWidth="1"/>
-    <col min="22" max="22" width="16.875" style="4" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.3984375" style="4" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="19.59765625" style="4" bestFit="1" customWidth="1"/>
+    <col min="20" max="21" width="19.59765625" style="4" customWidth="1"/>
+    <col min="22" max="22" width="16.8984375" style="4" bestFit="1" customWidth="1"/>
     <col min="23" max="24" width="24" style="4" customWidth="1"/>
-    <col min="25" max="26" width="28.375" style="4" bestFit="1" customWidth="1"/>
-    <col min="27" max="30" width="8.625" style="4"/>
-    <col min="31" max="31" width="9.25" style="4" bestFit="1" customWidth="1"/>
-    <col min="32" max="35" width="8.625" style="4"/>
-    <col min="36" max="36" width="13.625" style="11" bestFit="1" customWidth="1"/>
+    <col min="25" max="26" width="28.3984375" style="4" bestFit="1" customWidth="1"/>
+    <col min="27" max="30" width="8.59765625" style="4"/>
+    <col min="31" max="31" width="9.19921875" style="4" bestFit="1" customWidth="1"/>
+    <col min="32" max="35" width="8.59765625" style="4"/>
+    <col min="36" max="36" width="13.59765625" style="11" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="11" style="11" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="13.625" style="11" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="9.625" style="11" bestFit="1" customWidth="1"/>
-    <col min="40" max="16384" width="8.625" style="4"/>
+    <col min="38" max="38" width="13.59765625" style="11" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="9.59765625" style="11" bestFit="1" customWidth="1"/>
+    <col min="40" max="16384" width="8.59765625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:39" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="62"/>
       <c r="B1" s="4"/>
       <c r="O1" s="62"/>
@@ -17030,21 +17030,21 @@
       <c r="X1" s="69"/>
       <c r="Y1" s="70"/>
       <c r="Z1" s="70"/>
-      <c r="AA1" s="436" t="s">
+      <c r="AA1" s="438" t="s">
         <v>12</v>
       </c>
-      <c r="AB1" s="436"/>
-      <c r="AC1" s="436"/>
-      <c r="AD1" s="436" t="s">
+      <c r="AB1" s="438"/>
+      <c r="AC1" s="438"/>
+      <c r="AD1" s="438" t="s">
         <v>13</v>
       </c>
-      <c r="AE1" s="436"/>
-      <c r="AF1" s="436"/>
-      <c r="AG1" s="436" t="s">
+      <c r="AE1" s="438"/>
+      <c r="AF1" s="438"/>
+      <c r="AG1" s="438" t="s">
         <v>14</v>
       </c>
-      <c r="AH1" s="436"/>
-      <c r="AI1" s="436"/>
+      <c r="AH1" s="438"/>
+      <c r="AI1" s="438"/>
       <c r="AJ1" s="105" t="s">
         <v>136</v>
       </c>
@@ -17058,7 +17058,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="2" spans="1:39" s="25" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:39" s="25" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A2" s="253" t="s">
         <v>71</v>
       </c>
@@ -17177,7 +17177,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="3" spans="1:39" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:39" s="2" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A3" s="254" t="s">
         <v>35</v>
       </c>
@@ -17273,7 +17273,7 @@
       <c r="AL3" s="293"/>
       <c r="AM3" s="294"/>
     </row>
-    <row r="4" spans="1:39" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:39" s="2" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A4" s="243" t="s">
         <v>35</v>
       </c>
@@ -17370,7 +17370,7 @@
       <c r="AL4" s="293"/>
       <c r="AM4" s="294"/>
     </row>
-    <row r="5" spans="1:39" s="2" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:39" s="2" customFormat="1" ht="69" x14ac:dyDescent="0.3">
       <c r="A5" s="243" t="s">
         <v>35</v>
       </c>
@@ -17466,7 +17466,7 @@
       <c r="AL5" s="293"/>
       <c r="AM5" s="294"/>
     </row>
-    <row r="6" spans="1:39" s="2" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:39" s="2" customFormat="1" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A6" s="243" t="s">
         <v>35</v>
       </c>
@@ -17563,7 +17563,7 @@
       <c r="AL6" s="293"/>
       <c r="AM6" s="294"/>
     </row>
-    <row r="7" spans="1:39" s="2" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:39" s="2" customFormat="1" ht="69" x14ac:dyDescent="0.3">
       <c r="A7" s="243" t="s">
         <v>35</v>
       </c>
@@ -17660,7 +17660,7 @@
       <c r="AL7" s="293"/>
       <c r="AM7" s="294"/>
     </row>
-    <row r="8" spans="1:39" s="2" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:39" s="2" customFormat="1" ht="69" x14ac:dyDescent="0.3">
       <c r="A8" s="243" t="s">
         <v>35</v>
       </c>
@@ -17757,7 +17757,7 @@
       <c r="AL8" s="293"/>
       <c r="AM8" s="294"/>
     </row>
-    <row r="9" spans="1:39" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:39" s="2" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A9" s="243" t="s">
         <v>35</v>
       </c>
@@ -17854,7 +17854,7 @@
       <c r="AL9" s="293"/>
       <c r="AM9" s="294"/>
     </row>
-    <row r="10" spans="1:39" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:39" s="2" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A10" s="243" t="s">
         <v>35</v>
       </c>
@@ -17951,7 +17951,7 @@
       <c r="AL10" s="293"/>
       <c r="AM10" s="294"/>
     </row>
-    <row r="11" spans="1:39" s="2" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:39" s="2" customFormat="1" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A11" s="316" t="s">
         <v>35</v>
       </c>
@@ -18054,7 +18054,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:39" s="2" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:39" s="2" customFormat="1" ht="82.8" x14ac:dyDescent="0.3">
       <c r="A12" s="243" t="s">
         <v>179</v>
       </c>
@@ -18148,7 +18148,7 @@
       <c r="AL12" s="293"/>
       <c r="AM12" s="294"/>
     </row>
-    <row r="13" spans="1:39" s="2" customFormat="1" ht="242.25" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:39" s="2" customFormat="1" ht="262.2" x14ac:dyDescent="0.3">
       <c r="A13" s="199" t="s">
         <v>179</v>
       </c>
@@ -18188,7 +18188,7 @@
       <c r="N13" s="100"/>
       <c r="O13" s="47"/>
       <c r="P13" s="47" t="s">
-        <v>1005</v>
+        <v>1003</v>
       </c>
       <c r="Q13" s="6">
         <v>2</v>
@@ -18218,7 +18218,7 @@
       <c r="AL13" s="293"/>
       <c r="AM13" s="294"/>
     </row>
-    <row r="14" spans="1:39" s="2" customFormat="1" ht="165.75" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:39" s="2" customFormat="1" ht="179.4" x14ac:dyDescent="0.3">
       <c r="A14" s="254" t="s">
         <v>34</v>
       </c>
@@ -18315,7 +18315,7 @@
       <c r="AL14" s="74"/>
       <c r="AM14" s="74"/>
     </row>
-    <row r="15" spans="1:39" s="2" customFormat="1" ht="165.75" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:39" s="2" customFormat="1" ht="179.4" x14ac:dyDescent="0.3">
       <c r="A15" s="243" t="s">
         <v>34</v>
       </c>
@@ -18412,7 +18412,7 @@
       <c r="AL15" s="74"/>
       <c r="AM15" s="74"/>
     </row>
-    <row r="16" spans="1:39" s="2" customFormat="1" ht="165.75" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:39" s="2" customFormat="1" ht="179.4" x14ac:dyDescent="0.3">
       <c r="A16" s="243" t="s">
         <v>34</v>
       </c>
@@ -18509,7 +18509,7 @@
       <c r="AL16" s="74"/>
       <c r="AM16" s="74"/>
     </row>
-    <row r="17" spans="1:39" s="2" customFormat="1" ht="165.75" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:39" s="2" customFormat="1" ht="179.4" x14ac:dyDescent="0.3">
       <c r="A17" s="243" t="s">
         <v>34</v>
       </c>
@@ -18604,7 +18604,7 @@
       <c r="AL17" s="74"/>
       <c r="AM17" s="74"/>
     </row>
-    <row r="18" spans="1:39" s="2" customFormat="1" ht="114.75" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:39" s="2" customFormat="1" ht="124.2" x14ac:dyDescent="0.3">
       <c r="A18" s="243" t="s">
         <v>34</v>
       </c>
@@ -18701,7 +18701,7 @@
       <c r="AL18" s="74"/>
       <c r="AM18" s="74"/>
     </row>
-    <row r="19" spans="1:39" s="2" customFormat="1" ht="114.75" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:39" s="2" customFormat="1" ht="124.2" x14ac:dyDescent="0.3">
       <c r="A19" s="243" t="s">
         <v>34</v>
       </c>
@@ -18796,7 +18796,7 @@
       <c r="AL19" s="74"/>
       <c r="AM19" s="74"/>
     </row>
-    <row r="20" spans="1:39" s="76" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:39" s="76" customFormat="1" ht="82.8" x14ac:dyDescent="0.3">
       <c r="A20" s="255" t="s">
         <v>34</v>
       </c>
@@ -18892,7 +18892,7 @@
       <c r="AL20" s="75"/>
       <c r="AM20" s="75"/>
     </row>
-    <row r="21" spans="1:39" s="76" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:39" s="76" customFormat="1" ht="82.8" x14ac:dyDescent="0.3">
       <c r="A21" s="255" t="s">
         <v>34</v>
       </c>
@@ -18987,7 +18987,7 @@
       <c r="AL21" s="75"/>
       <c r="AM21" s="75"/>
     </row>
-    <row r="22" spans="1:39" s="76" customFormat="1" ht="178.5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:39" s="76" customFormat="1" ht="248.4" x14ac:dyDescent="0.3">
       <c r="A22" s="255" t="s">
         <v>34</v>
       </c>
@@ -19086,7 +19086,7 @@
       <c r="AL22" s="75"/>
       <c r="AM22" s="75"/>
     </row>
-    <row r="23" spans="1:39" s="76" customFormat="1" ht="178.5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:39" s="76" customFormat="1" ht="248.4" x14ac:dyDescent="0.3">
       <c r="A23" s="255" t="s">
         <v>34</v>
       </c>
@@ -19185,7 +19185,7 @@
       <c r="AL23" s="75"/>
       <c r="AM23" s="75"/>
     </row>
-    <row r="24" spans="1:39" ht="178.5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:39" ht="248.4" x14ac:dyDescent="0.3">
       <c r="A24" s="255" t="s">
         <v>34</v>
       </c>
@@ -19284,7 +19284,7 @@
       <c r="AL24" s="74"/>
       <c r="AM24" s="74"/>
     </row>
-    <row r="25" spans="1:39" ht="89.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:39" ht="89.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="255" t="s">
         <v>180</v>
       </c>
@@ -19377,7 +19377,7 @@
       <c r="AL25" s="74"/>
       <c r="AM25" s="74"/>
     </row>
-    <row r="26" spans="1:39" s="76" customFormat="1" ht="165.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:39" s="76" customFormat="1" ht="165.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="255" t="s">
         <v>180</v>
       </c>
@@ -19470,7 +19470,7 @@
       <c r="AL26" s="57"/>
       <c r="AM26" s="281"/>
     </row>
-    <row r="27" spans="1:39" s="76" customFormat="1" ht="204" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:39" s="76" customFormat="1" ht="204" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="255" t="s">
         <v>180</v>
       </c>
@@ -19543,7 +19543,7 @@
       <c r="AL27" s="57"/>
       <c r="AM27" s="281"/>
     </row>
-    <row r="28" spans="1:39" s="76" customFormat="1" ht="153" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:39" s="76" customFormat="1" ht="165.6" x14ac:dyDescent="0.3">
       <c r="A28" s="259" t="s">
         <v>180</v>
       </c>
@@ -19617,7 +19617,7 @@
       <c r="AL28" s="57"/>
       <c r="AM28" s="281"/>
     </row>
-    <row r="29" spans="1:39" s="76" customFormat="1" ht="153" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:39" s="76" customFormat="1" ht="165.6" x14ac:dyDescent="0.3">
       <c r="A29" s="259" t="s">
         <v>180</v>
       </c>
@@ -19692,7 +19692,7 @@
       <c r="AL29" s="57"/>
       <c r="AM29" s="281"/>
     </row>
-    <row r="30" spans="1:39" s="76" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:39" s="76" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A30" s="259" t="s">
         <v>35</v>
       </c>
@@ -19768,7 +19768,7 @@
       <c r="AL30" s="57"/>
       <c r="AM30" s="281"/>
     </row>
-    <row r="31" spans="1:39" s="76" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:39" s="76" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A31" s="259" t="s">
         <v>35</v>
       </c>
@@ -19845,7 +19845,7 @@
       <c r="AL31" s="57"/>
       <c r="AM31" s="281"/>
     </row>
-    <row r="32" spans="1:39" s="76" customFormat="1" ht="153" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:39" s="76" customFormat="1" ht="165.6" x14ac:dyDescent="0.3">
       <c r="A32" s="259" t="s">
         <v>35</v>
       </c>
@@ -19890,7 +19890,7 @@
         <v>754</v>
       </c>
       <c r="P32" s="417" t="s">
-        <v>1006</v>
+        <v>1004</v>
       </c>
       <c r="Q32" s="6">
         <v>2</v>
@@ -19922,7 +19922,7 @@
       <c r="AL32" s="57"/>
       <c r="AM32" s="281"/>
     </row>
-    <row r="33" spans="1:39" s="76" customFormat="1" ht="165.75" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:39" s="76" customFormat="1" ht="179.4" x14ac:dyDescent="0.3">
       <c r="A33" s="259" t="s">
         <v>35</v>
       </c>
@@ -19967,7 +19967,7 @@
         <v>818</v>
       </c>
       <c r="P33" s="416" t="s">
-        <v>1007</v>
+        <v>1005</v>
       </c>
       <c r="Q33" s="6">
         <v>2</v>
@@ -19999,7 +19999,7 @@
       <c r="AL33" s="57"/>
       <c r="AM33" s="281"/>
     </row>
-    <row r="34" spans="1:39" s="76" customFormat="1" ht="82.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:39" s="76" customFormat="1" ht="82.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="259" t="s">
         <v>34</v>
       </c>
@@ -20076,7 +20076,7 @@
       <c r="AL34" s="57"/>
       <c r="AM34" s="281"/>
     </row>
-    <row r="35" spans="1:39" s="76" customFormat="1" ht="82.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:39" s="76" customFormat="1" ht="82.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="259" t="s">
         <v>34</v>
       </c>
@@ -20153,7 +20153,7 @@
       <c r="AL35" s="57"/>
       <c r="AM35" s="281"/>
     </row>
-    <row r="36" spans="1:39" s="76" customFormat="1" ht="82.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:39" s="76" customFormat="1" ht="82.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="259" t="s">
         <v>34</v>
       </c>
@@ -20230,7 +20230,7 @@
       <c r="AL36" s="57"/>
       <c r="AM36" s="281"/>
     </row>
-    <row r="37" spans="1:39" s="76" customFormat="1" ht="102" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:39" s="76" customFormat="1" ht="102" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="259" t="s">
         <v>34</v>
       </c>
@@ -20277,7 +20277,7 @@
         <v>812</v>
       </c>
       <c r="P37" s="418" t="s">
-        <v>1008</v>
+        <v>1006</v>
       </c>
       <c r="Q37" s="6">
         <v>2</v>
@@ -20309,7 +20309,7 @@
       <c r="AL37" s="57"/>
       <c r="AM37" s="281"/>
     </row>
-    <row r="38" spans="1:39" s="76" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:39" s="76" customFormat="1" ht="82.8" x14ac:dyDescent="0.3">
       <c r="A38" s="259" t="s">
         <v>698</v>
       </c>
@@ -20386,7 +20386,7 @@
       <c r="AL38" s="57"/>
       <c r="AM38" s="281"/>
     </row>
-    <row r="39" spans="1:39" s="76" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:39" s="76" customFormat="1" ht="82.8" x14ac:dyDescent="0.3">
       <c r="A39" s="259" t="s">
         <v>698</v>
       </c>
@@ -20463,7 +20463,7 @@
       <c r="AL39" s="57"/>
       <c r="AM39" s="281"/>
     </row>
-    <row r="40" spans="1:39" s="76" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:39" s="76" customFormat="1" ht="82.8" x14ac:dyDescent="0.3">
       <c r="A40" s="259" t="s">
         <v>698</v>
       </c>
@@ -20540,7 +20540,7 @@
       <c r="AL40" s="57"/>
       <c r="AM40" s="281"/>
     </row>
-    <row r="41" spans="1:39" s="76" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:39" s="76" customFormat="1" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A41" s="259" t="s">
         <v>698</v>
       </c>
@@ -20587,7 +20587,7 @@
         <v>743</v>
       </c>
       <c r="P41" s="418" t="s">
-        <v>1009</v>
+        <v>1007</v>
       </c>
       <c r="Q41" s="6">
         <v>2</v>
@@ -20617,7 +20617,7 @@
       <c r="AL41" s="57"/>
       <c r="AM41" s="281"/>
     </row>
-    <row r="42" spans="1:39" s="76" customFormat="1" ht="204.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:39" s="76" customFormat="1" ht="221.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" s="259" t="s">
         <v>179</v>
       </c>
@@ -20662,7 +20662,7 @@
         <v>814</v>
       </c>
       <c r="P42" s="419" t="s">
-        <v>1010</v>
+        <v>1008</v>
       </c>
       <c r="Q42" s="6">
         <v>2</v>
@@ -20694,7 +20694,7 @@
       <c r="AL42" s="57"/>
       <c r="AM42" s="281"/>
     </row>
-    <row r="43" spans="1:39" s="76" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:39" s="76" customFormat="1" ht="96.6" x14ac:dyDescent="0.3">
       <c r="A43" s="259" t="s">
         <v>179</v>
       </c>
@@ -20769,7 +20769,7 @@
       <c r="AL43" s="57"/>
       <c r="AM43" s="281"/>
     </row>
-    <row r="44" spans="1:39" s="76" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:39" s="76" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="259" t="s">
         <v>180</v>
       </c>
@@ -20844,7 +20844,7 @@
       <c r="AL44" s="57"/>
       <c r="AM44" s="281"/>
     </row>
-    <row r="45" spans="1:39" s="76" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:39" s="76" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="259" t="s">
         <v>519</v>
       </c>
@@ -20889,7 +20889,7 @@
         <v>815</v>
       </c>
       <c r="P45" s="418" t="s">
-        <v>1011</v>
+        <v>1009</v>
       </c>
       <c r="Q45" s="6">
         <v>2</v>
@@ -20919,7 +20919,7 @@
       <c r="AL45" s="57"/>
       <c r="AM45" s="281"/>
     </row>
-    <row r="46" spans="1:39" s="76" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:39" s="76" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="259" t="s">
         <v>519</v>
       </c>
@@ -20996,7 +20996,7 @@
       <c r="AL46" s="57"/>
       <c r="AM46" s="281"/>
     </row>
-    <row r="47" spans="1:39" s="76" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:39" s="76" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="259" t="s">
         <v>605</v>
       </c>
@@ -21043,7 +21043,7 @@
         <v>816</v>
       </c>
       <c r="P47" s="418" t="s">
-        <v>1012</v>
+        <v>1010</v>
       </c>
       <c r="Q47" s="6">
         <v>2</v>
@@ -21073,7 +21073,7 @@
       <c r="AL47" s="57"/>
       <c r="AM47" s="281"/>
     </row>
-    <row r="48" spans="1:39" s="76" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:39" s="76" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="259" t="s">
         <v>605</v>
       </c>
@@ -21150,7 +21150,7 @@
       <c r="AL48" s="57"/>
       <c r="AM48" s="281"/>
     </row>
-    <row r="49" spans="1:39" s="76" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:39" s="76" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="259" t="s">
         <v>606</v>
       </c>
@@ -21197,7 +21197,7 @@
         <v>817</v>
       </c>
       <c r="P49" s="418" t="s">
-        <v>1013</v>
+        <v>1011</v>
       </c>
       <c r="Q49" s="6">
         <v>2</v>
@@ -21227,7 +21227,7 @@
       <c r="AL49" s="57"/>
       <c r="AM49" s="281"/>
     </row>
-    <row r="50" spans="1:39" s="76" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:39" s="76" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="259" t="s">
         <v>606</v>
       </c>
@@ -21304,7 +21304,7 @@
       <c r="AL50" s="57"/>
       <c r="AM50" s="281"/>
     </row>
-    <row r="51" spans="1:39" s="76" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:39" s="76" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="259" t="s">
         <v>355</v>
       </c>
@@ -21379,7 +21379,7 @@
       <c r="AL51" s="57"/>
       <c r="AM51" s="281"/>
     </row>
-    <row r="52" spans="1:39" s="76" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:39" s="76" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="259" t="s">
         <v>551</v>
       </c>
@@ -21424,7 +21424,7 @@
         <v>905</v>
       </c>
       <c r="P52" s="418" t="s">
-        <v>1014</v>
+        <v>1012</v>
       </c>
       <c r="Q52" s="6">
         <v>2</v>
@@ -21454,7 +21454,7 @@
       <c r="AL52" s="57"/>
       <c r="AM52" s="281"/>
     </row>
-    <row r="53" spans="1:39" s="76" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:39" s="76" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="259" t="s">
         <v>551</v>
       </c>
@@ -21529,7 +21529,7 @@
       <c r="AL53" s="57"/>
       <c r="AM53" s="281"/>
     </row>
-    <row r="54" spans="1:39" s="76" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:39" s="76" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="259" t="s">
         <v>557</v>
       </c>
@@ -21669,80 +21669,80 @@
       <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.625" style="25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.375" style="13" customWidth="1"/>
+    <col min="1" max="1" width="16.59765625" style="25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.3984375" style="13" customWidth="1"/>
     <col min="3" max="3" width="14" style="4" customWidth="1"/>
-    <col min="4" max="4" width="33.25" style="25" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.875" style="27" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.25" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.625" style="27" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="98.875" style="31" customWidth="1"/>
-    <col min="9" max="9" width="38.375" style="45" customWidth="1"/>
+    <col min="4" max="4" width="33.19921875" style="25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.8984375" style="27" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.19921875" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.59765625" style="27" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="98.8984375" style="31" customWidth="1"/>
+    <col min="9" max="9" width="38.3984375" style="45" customWidth="1"/>
     <col min="10" max="10" width="36.5" style="45" customWidth="1"/>
-    <col min="11" max="12" width="17.125" style="31" customWidth="1"/>
-    <col min="13" max="13" width="25.875" style="27" customWidth="1"/>
-    <col min="14" max="14" width="77.875" style="4" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="43.625" style="49" customWidth="1"/>
-    <col min="16" max="17" width="13.125" style="8" customWidth="1"/>
-    <col min="18" max="18" width="15.625" style="8" customWidth="1"/>
-    <col min="19" max="19" width="17.125" style="8" customWidth="1"/>
-    <col min="20" max="21" width="22.375" style="8" customWidth="1"/>
-    <col min="22" max="22" width="17.375" style="9" customWidth="1"/>
-    <col min="23" max="23" width="29.125" style="9" customWidth="1"/>
+    <col min="11" max="12" width="17.09765625" style="31" customWidth="1"/>
+    <col min="13" max="13" width="25.8984375" style="27" customWidth="1"/>
+    <col min="14" max="14" width="77.8984375" style="4" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="43.59765625" style="49" customWidth="1"/>
+    <col min="16" max="17" width="13.09765625" style="8" customWidth="1"/>
+    <col min="18" max="18" width="15.59765625" style="8" customWidth="1"/>
+    <col min="19" max="19" width="17.09765625" style="8" customWidth="1"/>
+    <col min="20" max="21" width="22.3984375" style="8" customWidth="1"/>
+    <col min="22" max="22" width="17.3984375" style="9" customWidth="1"/>
+    <col min="23" max="23" width="29.09765625" style="9" customWidth="1"/>
     <col min="24" max="24" width="15" style="11" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="11.5" style="11" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="15" style="11" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="13" style="11" customWidth="1"/>
     <col min="28" max="30" width="11.5" style="11" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="12.875" style="11" customWidth="1"/>
+    <col min="31" max="31" width="12.8984375" style="11" customWidth="1"/>
     <col min="32" max="34" width="15" style="11" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="11.5" style="40" customWidth="1"/>
-    <col min="36" max="38" width="12.125" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="10.125" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="11.625" style="12" customWidth="1"/>
-    <col min="41" max="41" width="21.125" style="12" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="19.625" style="12" bestFit="1" customWidth="1"/>
-    <col min="43" max="16384" width="8.625" style="3"/>
+    <col min="36" max="38" width="12.09765625" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="10.09765625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="11.59765625" style="12" customWidth="1"/>
+    <col min="41" max="41" width="21.09765625" style="12" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="19.59765625" style="12" bestFit="1" customWidth="1"/>
+    <col min="43" max="16384" width="8.59765625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:42" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B1" s="3"/>
       <c r="O1" s="27"/>
       <c r="V1" s="10"/>
       <c r="W1" s="10"/>
-      <c r="X1" s="431" t="s">
+      <c r="X1" s="433" t="s">
         <v>12</v>
       </c>
-      <c r="Y1" s="432"/>
-      <c r="Z1" s="432"/>
-      <c r="AA1" s="433"/>
-      <c r="AB1" s="431" t="s">
+      <c r="Y1" s="434"/>
+      <c r="Z1" s="434"/>
+      <c r="AA1" s="435"/>
+      <c r="AB1" s="433" t="s">
         <v>13</v>
       </c>
-      <c r="AC1" s="432"/>
-      <c r="AD1" s="432"/>
-      <c r="AE1" s="433"/>
-      <c r="AF1" s="434" t="s">
+      <c r="AC1" s="434"/>
+      <c r="AD1" s="434"/>
+      <c r="AE1" s="435"/>
+      <c r="AF1" s="436" t="s">
         <v>14</v>
       </c>
-      <c r="AG1" s="435"/>
-      <c r="AH1" s="435"/>
-      <c r="AI1" s="435"/>
-      <c r="AJ1" s="434" t="s">
+      <c r="AG1" s="437"/>
+      <c r="AH1" s="437"/>
+      <c r="AI1" s="437"/>
+      <c r="AJ1" s="436" t="s">
         <v>68</v>
       </c>
-      <c r="AK1" s="435"/>
-      <c r="AL1" s="435"/>
-      <c r="AM1" s="435"/>
+      <c r="AK1" s="437"/>
+      <c r="AL1" s="437"/>
+      <c r="AM1" s="437"/>
       <c r="AN1" s="38"/>
-      <c r="AO1" s="442" t="s">
+      <c r="AO1" s="444" t="s">
         <v>20</v>
       </c>
-      <c r="AP1" s="442"/>
-    </row>
-    <row r="2" spans="1:42" s="46" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="AP1" s="444"/>
+    </row>
+    <row r="2" spans="1:42" s="46" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A2" s="44" t="s">
         <v>71</v>
       </c>
@@ -21908,49 +21908,49 @@
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="63.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="49.875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="156.125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="44.125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="32.625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="22.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.59765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="63.3984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.09765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="49.8984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.59765625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.59765625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.8984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="156.09765625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="44.09765625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="32.59765625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.8984375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.59765625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="22.09765625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="33" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="26.5" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="4" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="3.625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="3.59765625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="4" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="3.625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="3.59765625" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="4" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="16.875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="16.8984375" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="16" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="24" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="5.125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="5.09765625" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="37.5" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="14" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="10.375" bestFit="1" customWidth="1"/>
-    <col min="28" max="29" width="7.125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="9.625" bestFit="1" customWidth="1"/>
-    <col min="31" max="33" width="7.125" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="9.625" bestFit="1" customWidth="1"/>
-    <col min="35" max="37" width="7.125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="10.3984375" bestFit="1" customWidth="1"/>
+    <col min="28" max="29" width="7.09765625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="9.59765625" bestFit="1" customWidth="1"/>
+    <col min="31" max="33" width="7.09765625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="9.59765625" bestFit="1" customWidth="1"/>
+    <col min="35" max="37" width="7.09765625" bestFit="1" customWidth="1"/>
     <col min="38" max="38" width="10" bestFit="1" customWidth="1"/>
-    <col min="39" max="41" width="7.125" bestFit="1" customWidth="1"/>
+    <col min="39" max="41" width="7.09765625" bestFit="1" customWidth="1"/>
     <col min="42" max="42" width="10" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="26.125" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="20.625" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="21.875" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="26.09765625" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="20.59765625" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="21.8984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:46" s="98" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:46" s="98" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="92" t="s">
         <v>71</v>
       </c>
@@ -22087,7 +22087,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:46" s="89" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:46" s="89" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="133" t="s">
         <v>72</v>
       </c>
@@ -22169,7 +22169,7 @@
       <c r="AK2" s="87"/>
       <c r="AL2" s="87"/>
     </row>
-    <row r="3" spans="1:46" s="89" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:46" s="89" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="133" t="s">
         <v>72</v>
       </c>
@@ -22251,7 +22251,7 @@
       <c r="AK3" s="87"/>
       <c r="AL3" s="87"/>
     </row>
-    <row r="4" spans="1:46" s="89" customFormat="1" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:46" s="89" customFormat="1" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="107" t="s">
         <v>72</v>
       </c>
@@ -22339,7 +22339,7 @@
       <c r="AR4" s="144"/>
       <c r="AS4" s="144"/>
     </row>
-    <row r="5" spans="1:46" s="126" customFormat="1" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:46" s="126" customFormat="1" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="157" t="s">
         <v>72</v>
       </c>
@@ -22430,7 +22430,7 @@
       <c r="AS5" s="152"/>
       <c r="AT5" s="125"/>
     </row>
-    <row r="6" spans="1:46" s="126" customFormat="1" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:46" s="126" customFormat="1" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="107" t="s">
         <v>72</v>
       </c>
@@ -22521,7 +22521,7 @@
       <c r="AS6" s="152"/>
       <c r="AT6" s="125"/>
     </row>
-    <row r="7" spans="1:46" s="126" customFormat="1" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:46" s="126" customFormat="1" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="133" t="s">
         <v>72</v>
       </c>
@@ -22643,7 +22643,7 @@
       <c r="AS7" s="145"/>
       <c r="AT7" s="125"/>
     </row>
-    <row r="9" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A9" s="135"/>
       <c r="B9" t="s">
         <v>148</v>
@@ -22715,34 +22715,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G65"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="A60" sqref="A60"/>
+    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="91.75" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="62.75" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="32.75" style="317" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.625" style="217" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="91.69921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.3984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.8984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.3984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="62.69921875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="32.69921875" style="317" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.59765625" style="217" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.09765625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="161" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="135" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="160" t="s">
         <v>178</v>
       </c>
@@ -22765,9 +22765,9 @@
         <v>409</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="412" t="s">
-        <v>944</v>
+        <v>942</v>
       </c>
       <c r="B5" t="s">
         <v>72</v>
@@ -22786,9 +22786,9 @@
         <v>410</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="412" t="s">
-        <v>945</v>
+        <v>943</v>
       </c>
       <c r="B6" t="s">
         <v>72</v>
@@ -22807,9 +22807,9 @@
         <v>410</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="412" t="s">
-        <v>946</v>
+        <v>944</v>
       </c>
       <c r="B7" t="s">
         <v>72</v>
@@ -22828,9 +22828,9 @@
         <v>410</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="412" t="s">
-        <v>947</v>
+        <v>945</v>
       </c>
       <c r="B8" t="s">
         <v>72</v>
@@ -22849,9 +22849,9 @@
         <v>410</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="412" t="s">
-        <v>948</v>
+        <v>946</v>
       </c>
       <c r="B9" t="s">
         <v>72</v>
@@ -22870,9 +22870,9 @@
         <v>410</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="412" t="s">
-        <v>949</v>
+        <v>947</v>
       </c>
       <c r="B10" t="s">
         <v>72</v>
@@ -22884,14 +22884,14 @@
         <v>417</v>
       </c>
       <c r="E10" s="403" t="s">
-        <v>943</v>
+        <v>941</v>
       </c>
       <c r="F10" s="402"/>
       <c r="G10"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="412" t="s">
-        <v>950</v>
+        <v>948</v>
       </c>
       <c r="B11" t="s">
         <v>72</v>
@@ -22903,14 +22903,14 @@
         <v>417</v>
       </c>
       <c r="E11" s="404" t="s">
-        <v>940</v>
+        <v>938</v>
       </c>
       <c r="F11" s="402"/>
       <c r="G11"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="412" t="s">
-        <v>951</v>
+        <v>949</v>
       </c>
       <c r="B12" t="s">
         <v>72</v>
@@ -22922,14 +22922,14 @@
         <v>417</v>
       </c>
       <c r="E12" s="404" t="s">
-        <v>939</v>
+        <v>937</v>
       </c>
       <c r="F12" s="402"/>
       <c r="G12"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="412" t="s">
-        <v>952</v>
+        <v>950</v>
       </c>
       <c r="B13" t="s">
         <v>72</v>
@@ -22941,14 +22941,14 @@
         <v>417</v>
       </c>
       <c r="E13" s="404" t="s">
-        <v>938</v>
+        <v>936</v>
       </c>
       <c r="F13" s="402"/>
       <c r="G13"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="412" t="s">
-        <v>953</v>
+        <v>951</v>
       </c>
       <c r="B14" t="s">
         <v>72</v>
@@ -22960,14 +22960,14 @@
         <v>417</v>
       </c>
       <c r="E14" s="405" t="s">
-        <v>937</v>
+        <v>935</v>
       </c>
       <c r="F14" s="402"/>
       <c r="G14"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="412" t="s">
-        <v>954</v>
+        <v>952</v>
       </c>
       <c r="B15" t="s">
         <v>72</v>
@@ -22979,14 +22979,14 @@
         <v>417</v>
       </c>
       <c r="E15" s="403" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
       <c r="F15" s="402"/>
       <c r="G15"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="412" t="s">
-        <v>969</v>
+        <v>967</v>
       </c>
       <c r="B16" t="s">
         <v>72</v>
@@ -22998,16 +22998,16 @@
         <v>417</v>
       </c>
       <c r="E16" s="192" t="s">
-        <v>941</v>
+        <v>939</v>
       </c>
       <c r="F16" s="219"/>
       <c r="G16" s="220" t="s">
         <v>410</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="412" t="s">
-        <v>955</v>
+        <v>953</v>
       </c>
       <c r="B17" t="s">
         <v>72</v>
@@ -23026,9 +23026,9 @@
         <v>410</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="412" t="s">
-        <v>956</v>
+        <v>954</v>
       </c>
       <c r="B18" t="s">
         <v>72</v>
@@ -23047,9 +23047,9 @@
         <v>410</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="412" t="s">
-        <v>957</v>
+        <v>955</v>
       </c>
       <c r="B19" t="s">
         <v>72</v>
@@ -23068,9 +23068,9 @@
         <v>410</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="412" t="s">
-        <v>958</v>
+        <v>956</v>
       </c>
       <c r="B20" t="s">
         <v>72</v>
@@ -23089,9 +23089,9 @@
         <v>410</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="412" t="s">
-        <v>959</v>
+        <v>957</v>
       </c>
       <c r="B21" t="s">
         <v>72</v>
@@ -23110,9 +23110,9 @@
         <v>410</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="412" t="s">
-        <v>960</v>
+        <v>958</v>
       </c>
       <c r="B22" t="s">
         <v>72</v>
@@ -23131,9 +23131,9 @@
         <v>410</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="412" t="s">
-        <v>961</v>
+        <v>959</v>
       </c>
       <c r="B23" t="s">
         <v>72</v>
@@ -23145,14 +23145,14 @@
         <v>417</v>
       </c>
       <c r="E23" s="403" t="s">
-        <v>934</v>
+        <v>932</v>
       </c>
       <c r="F23" s="402"/>
       <c r="G23"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="412" t="s">
-        <v>962</v>
+        <v>960</v>
       </c>
       <c r="B24" t="s">
         <v>72</v>
@@ -23171,9 +23171,9 @@
         <v>410</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="412" t="s">
-        <v>963</v>
+        <v>961</v>
       </c>
       <c r="B25" t="s">
         <v>72</v>
@@ -23192,9 +23192,9 @@
         <v>410</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="413" t="s">
-        <v>964</v>
+        <v>962</v>
       </c>
       <c r="B26" t="s">
         <v>72</v>
@@ -23213,9 +23213,9 @@
         <v>410</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="413" t="s">
-        <v>965</v>
+        <v>963</v>
       </c>
       <c r="B27" t="s">
         <v>72</v>
@@ -23234,9 +23234,9 @@
         <v>410</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="413" t="s">
-        <v>966</v>
+        <v>964</v>
       </c>
       <c r="B28" t="s">
         <v>72</v>
@@ -23248,14 +23248,14 @@
         <v>417</v>
       </c>
       <c r="E28" s="403" t="s">
-        <v>935</v>
+        <v>933</v>
       </c>
       <c r="F28" s="402"/>
       <c r="G28"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="413" t="s">
-        <v>967</v>
+        <v>965</v>
       </c>
       <c r="B29" t="s">
         <v>72</v>
@@ -23274,9 +23274,9 @@
         <v>410</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="413" t="s">
-        <v>968</v>
+        <v>966</v>
       </c>
       <c r="B30" t="s">
         <v>72</v>
@@ -23288,14 +23288,14 @@
         <v>417</v>
       </c>
       <c r="E30" s="405" t="s">
-        <v>936</v>
+        <v>934</v>
       </c>
       <c r="F30" s="402"/>
       <c r="G30"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="413" t="s">
-        <v>1002</v>
+        <v>1000</v>
       </c>
       <c r="B31" t="s">
         <v>72</v>
@@ -23307,14 +23307,14 @@
         <v>417</v>
       </c>
       <c r="E31" s="405" t="s">
-        <v>1001</v>
+        <v>999</v>
       </c>
       <c r="F31" s="402"/>
       <c r="G31"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="413" t="s">
-        <v>970</v>
+        <v>968</v>
       </c>
       <c r="B32" t="s">
         <v>72</v>
@@ -23333,9 +23333,9 @@
         <v>410</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="413" t="s">
-        <v>971</v>
+        <v>969</v>
       </c>
       <c r="B33" t="s">
         <v>72</v>
@@ -23354,9 +23354,9 @@
         <v>410</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="413" t="s">
-        <v>1015</v>
+        <v>1013</v>
       </c>
       <c r="B34" t="s">
         <v>72</v>
@@ -23368,12 +23368,12 @@
         <v>406</v>
       </c>
       <c r="E34" s="192" t="s">
-        <v>1016</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+        <v>1014</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="413" t="s">
-        <v>1017</v>
+        <v>1015</v>
       </c>
       <c r="B35" t="s">
         <v>72</v>
@@ -23385,12 +23385,12 @@
         <v>406</v>
       </c>
       <c r="E35" s="192" t="s">
-        <v>1018</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+        <v>1016</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="413" t="s">
-        <v>972</v>
+        <v>970</v>
       </c>
       <c r="B36" t="s">
         <v>907</v>
@@ -23409,9 +23409,9 @@
         <v>410</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="413" t="s">
-        <v>973</v>
+        <v>971</v>
       </c>
       <c r="B37" t="s">
         <v>907</v>
@@ -23430,9 +23430,9 @@
         <v>410</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="413" t="s">
-        <v>982</v>
+        <v>980</v>
       </c>
       <c r="B38" s="395" t="s">
         <v>519</v>
@@ -23444,15 +23444,15 @@
         <v>406</v>
       </c>
       <c r="E38" s="397" t="s">
-        <v>922</v>
+        <v>920</v>
       </c>
       <c r="G38" s="220" t="s">
         <v>410</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="413" t="s">
-        <v>983</v>
+        <v>981</v>
       </c>
       <c r="B39" s="395" t="s">
         <v>519</v>
@@ -23464,18 +23464,18 @@
         <v>407</v>
       </c>
       <c r="E39" s="397" t="s">
-        <v>921</v>
+        <v>919</v>
       </c>
       <c r="G39" s="220" t="s">
         <v>410</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="413" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
       <c r="B40" s="395" t="s">
-        <v>926</v>
+        <v>924</v>
       </c>
       <c r="C40" s="395" t="s">
         <v>911</v>
@@ -23484,18 +23484,18 @@
         <v>406</v>
       </c>
       <c r="E40" s="397" t="s">
-        <v>929</v>
+        <v>927</v>
       </c>
       <c r="G40" s="220" t="s">
         <v>410</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="413" t="s">
-        <v>988</v>
+        <v>986</v>
       </c>
       <c r="B41" s="395" t="s">
-        <v>926</v>
+        <v>924</v>
       </c>
       <c r="C41" s="395" t="s">
         <v>911</v>
@@ -23504,18 +23504,18 @@
         <v>407</v>
       </c>
       <c r="E41" s="397" t="s">
-        <v>927</v>
+        <v>925</v>
       </c>
       <c r="G41" s="220" t="s">
         <v>410</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="413" t="s">
-        <v>989</v>
+        <v>987</v>
       </c>
       <c r="B42" s="395" t="s">
-        <v>926</v>
+        <v>924</v>
       </c>
       <c r="C42" s="395" t="s">
         <v>911</v>
@@ -23524,15 +23524,15 @@
         <v>407</v>
       </c>
       <c r="E42" s="397" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="G42" s="220" t="s">
         <v>410</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" s="413" t="s">
-        <v>974</v>
+        <v>972</v>
       </c>
       <c r="B43" s="395" t="s">
         <v>910</v>
@@ -23544,15 +23544,15 @@
         <v>406</v>
       </c>
       <c r="E43" s="397" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="G43" s="220" t="s">
         <v>410</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" s="413" t="s">
-        <v>975</v>
+        <v>973</v>
       </c>
       <c r="B44" s="395" t="s">
         <v>910</v>
@@ -23564,15 +23564,15 @@
         <v>407</v>
       </c>
       <c r="E44" s="397" t="s">
-        <v>912</v>
+        <v>1056</v>
       </c>
       <c r="G44" s="220" t="s">
         <v>410</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" s="413" t="s">
-        <v>976</v>
+        <v>974</v>
       </c>
       <c r="B45" s="395" t="s">
         <v>910</v>
@@ -23584,12 +23584,12 @@
         <v>408</v>
       </c>
       <c r="E45" s="397" t="s">
-        <v>914</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+        <v>913</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" s="413" t="s">
-        <v>977</v>
+        <v>975</v>
       </c>
       <c r="B46" s="395" t="s">
         <v>910</v>
@@ -23601,15 +23601,15 @@
         <v>418</v>
       </c>
       <c r="E46" s="409" t="s">
+        <v>914</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A47" s="413" t="s">
+        <v>976</v>
+      </c>
+      <c r="B47" s="395" t="s">
         <v>915</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="413" t="s">
-        <v>978</v>
-      </c>
-      <c r="B47" s="395" t="s">
-        <v>916</v>
       </c>
       <c r="C47" s="395" t="s">
         <v>911</v>
@@ -23618,18 +23618,18 @@
         <v>406</v>
       </c>
       <c r="E47" s="397" t="s">
-        <v>918</v>
+        <v>916</v>
       </c>
       <c r="G47" s="220" t="s">
         <v>410</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="413" t="s">
-        <v>979</v>
+        <v>977</v>
       </c>
       <c r="B48" s="395" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="C48" s="395" t="s">
         <v>911</v>
@@ -23638,18 +23638,18 @@
         <v>407</v>
       </c>
       <c r="E48" s="397" t="s">
-        <v>917</v>
+        <v>1057</v>
       </c>
       <c r="G48" s="220" t="s">
         <v>410</v>
       </c>
     </row>
-    <row r="49" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="413" t="s">
-        <v>980</v>
+        <v>978</v>
       </c>
       <c r="B49" s="395" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="C49" s="395" t="s">
         <v>911</v>
@@ -23658,15 +23658,15 @@
         <v>408</v>
       </c>
       <c r="E49" s="397" t="s">
-        <v>919</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>917</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="413" t="s">
-        <v>981</v>
+        <v>979</v>
       </c>
       <c r="B50" s="395" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="C50" s="395" t="s">
         <v>911</v>
@@ -23675,12 +23675,12 @@
         <v>418</v>
       </c>
       <c r="E50" s="410" t="s">
-        <v>920</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+        <v>918</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" s="413" t="s">
-        <v>984</v>
+        <v>982</v>
       </c>
       <c r="B51" s="395" t="s">
         <v>355</v>
@@ -23692,15 +23692,15 @@
         <v>407</v>
       </c>
       <c r="E51" s="397" t="s">
-        <v>923</v>
+        <v>921</v>
       </c>
       <c r="G51" s="220" t="s">
         <v>410</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" s="413" t="s">
-        <v>985</v>
+        <v>983</v>
       </c>
       <c r="B52" s="395" t="s">
         <v>355</v>
@@ -23712,12 +23712,12 @@
         <v>408</v>
       </c>
       <c r="E52" s="397" t="s">
-        <v>924</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+        <v>922</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" s="413" t="s">
-        <v>986</v>
+        <v>984</v>
       </c>
       <c r="B53" s="395" t="s">
         <v>355</v>
@@ -23729,12 +23729,12 @@
         <v>418</v>
       </c>
       <c r="E53" s="410" t="s">
-        <v>925</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" s="413" t="s">
-        <v>990</v>
+        <v>988</v>
       </c>
       <c r="B54" s="395" t="s">
         <v>557</v>
@@ -23746,15 +23746,15 @@
         <v>406</v>
       </c>
       <c r="E54" s="397" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
       <c r="G54" s="220" t="s">
         <v>410</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" s="413" t="s">
-        <v>991</v>
+        <v>989</v>
       </c>
       <c r="B55" s="395" t="s">
         <v>557</v>
@@ -23766,15 +23766,15 @@
         <v>407</v>
       </c>
       <c r="E55" s="410" t="s">
-        <v>930</v>
+        <v>928</v>
       </c>
       <c r="G55" s="220" t="s">
         <v>410</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56" s="412" t="s">
-        <v>1000</v>
+        <v>998</v>
       </c>
       <c r="B56" t="s">
         <v>727</v>
@@ -23793,9 +23793,9 @@
         <v>410</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" s="412" t="s">
-        <v>992</v>
+        <v>990</v>
       </c>
       <c r="B57" t="s">
         <v>256</v>
@@ -23814,9 +23814,9 @@
         <v>410</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" s="412" t="s">
-        <v>993</v>
+        <v>991</v>
       </c>
       <c r="B58" t="s">
         <v>256</v>
@@ -23835,9 +23835,9 @@
         <v>410</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" s="421" t="s">
-        <v>994</v>
+        <v>992</v>
       </c>
       <c r="B59" s="408" t="s">
         <v>256</v>
@@ -23858,9 +23858,9 @@
         <v>410</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60" s="414" t="s">
-        <v>1056</v>
+        <v>1054</v>
       </c>
       <c r="B60" t="s">
         <v>263</v>
@@ -23872,14 +23872,14 @@
         <v>407</v>
       </c>
       <c r="E60" s="192" t="s">
-        <v>1055</v>
+        <v>1053</v>
       </c>
       <c r="F60" s="219"/>
       <c r="G60" s="220"/>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61" s="412" t="s">
-        <v>999</v>
+        <v>997</v>
       </c>
       <c r="B61" t="s">
         <v>909</v>
@@ -23898,9 +23898,9 @@
         <v>410</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" s="412" t="s">
-        <v>995</v>
+        <v>993</v>
       </c>
       <c r="B62" t="s">
         <v>908</v>
@@ -23917,9 +23917,9 @@
       <c r="F62" s="219"/>
       <c r="G62" s="220"/>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63" s="412" t="s">
-        <v>996</v>
+        <v>994</v>
       </c>
       <c r="B63" t="s">
         <v>908</v>
@@ -23936,9 +23936,9 @@
       <c r="F63" s="219"/>
       <c r="G63" s="220"/>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A64" s="412" t="s">
-        <v>997</v>
+        <v>995</v>
       </c>
       <c r="B64" t="s">
         <v>908</v>
@@ -23950,16 +23950,16 @@
         <v>406</v>
       </c>
       <c r="E64" s="192" t="s">
-        <v>932</v>
+        <v>930</v>
       </c>
       <c r="F64" s="219" t="s">
-        <v>1003</v>
+        <v>1001</v>
       </c>
       <c r="G64" s="220"/>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A65" s="421" t="s">
-        <v>998</v>
+        <v>996</v>
       </c>
       <c r="B65" t="s">
         <v>908</v>
@@ -24002,14 +24002,14 @@
       <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.25" style="154" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="8.875" style="156" customWidth="1"/>
-    <col min="6" max="7" width="8.875" customWidth="1"/>
+    <col min="1" max="1" width="18.19921875" style="154" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="8.8984375" style="156" customWidth="1"/>
+    <col min="6" max="7" width="8.8984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B1" s="360"/>
       <c r="C1" s="359"/>
       <c r="D1" s="163"/>
@@ -24017,8 +24017,8 @@
       <c r="F1" s="165"/>
       <c r="G1" s="166"/>
     </row>
-    <row r="2" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="162" t="s">
         <v>699</v>
       </c>
@@ -24026,172 +24026,172 @@
         <v>701</v>
       </c>
       <c r="C3" s="359" t="s">
-        <v>1041</v>
+        <v>1039</v>
       </c>
       <c r="D3" s="361" t="s">
-        <v>1022</v>
+        <v>1020</v>
       </c>
       <c r="E3"/>
     </row>
-    <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4"/>
       <c r="B4" s="360" t="s">
         <v>702</v>
       </c>
       <c r="C4" s="359" t="s">
-        <v>1042</v>
+        <v>1040</v>
       </c>
       <c r="D4" s="361" t="s">
         <v>718</v>
       </c>
       <c r="E4"/>
     </row>
-    <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5"/>
       <c r="B5" s="360" t="s">
         <v>703</v>
       </c>
       <c r="C5" s="359" t="s">
-        <v>1043</v>
+        <v>1041</v>
       </c>
       <c r="D5" s="361" t="s">
         <v>719</v>
       </c>
       <c r="E5"/>
     </row>
-    <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6"/>
       <c r="B6" s="360" t="s">
         <v>704</v>
       </c>
       <c r="C6" s="359" t="s">
-        <v>1044</v>
+        <v>1042</v>
       </c>
       <c r="D6" s="361" t="s">
-        <v>1023</v>
+        <v>1021</v>
       </c>
       <c r="E6"/>
     </row>
-    <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7"/>
       <c r="B7" s="360" t="s">
         <v>705</v>
       </c>
       <c r="C7" s="359" t="s">
-        <v>1045</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1043</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8"/>
       <c r="C8" s="359" t="s">
-        <v>1046</v>
+        <v>1044</v>
       </c>
       <c r="D8"/>
     </row>
-    <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9"/>
       <c r="C9" s="359" t="s">
         <v>717</v>
       </c>
       <c r="D9"/>
     </row>
-    <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10"/>
       <c r="C10" s="359" t="s">
         <v>706</v>
       </c>
       <c r="D10"/>
     </row>
-    <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11"/>
       <c r="C11" s="359" t="s">
         <v>707</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12"/>
       <c r="C12" s="359" t="s">
         <v>708</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13"/>
       <c r="C13" s="359" t="s">
         <v>709</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14"/>
       <c r="C14" s="359" t="s">
         <v>710</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15"/>
       <c r="C15" s="359" t="s">
         <v>711</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16"/>
       <c r="C16" s="359" t="s">
-        <v>1047</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1045</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17"/>
       <c r="C17" s="359" t="s">
         <v>712</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18"/>
       <c r="C18" s="359" t="s">
         <v>713</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19"/>
       <c r="C19" s="359" t="s">
         <v>714</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20"/>
       <c r="C20" s="359" t="s">
         <v>715</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21"/>
       <c r="C21" s="359" t="s">
-        <v>1048</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1046</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22"/>
       <c r="C22" s="359" t="s">
         <v>716</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23"/>
       <c r="C23" s="359" t="s">
-        <v>1049</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1047</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24"/>
       <c r="C24" s="359" t="s">
-        <v>1024</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1022</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25"/>
     </row>
-    <row r="26" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="162" t="s">
-        <v>1025</v>
+        <v>1023</v>
       </c>
       <c r="D26" s="361" t="s">
         <v>700</v>
@@ -24201,15 +24201,15 @@
       </c>
       <c r="G26" s="156"/>
     </row>
-    <row r="27" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27"/>
     </row>
-    <row r="28" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="162" t="s">
         <v>256</v>
       </c>
       <c r="C28" s="359" t="s">
-        <v>1024</v>
+        <v>1022</v>
       </c>
       <c r="D28" s="361" t="s">
         <v>721</v>
@@ -24221,111 +24221,111 @@
         <v>723</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29"/>
       <c r="B29"/>
       <c r="C29"/>
       <c r="D29"/>
       <c r="E29"/>
     </row>
-    <row r="30" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="162" t="s">
         <v>519</v>
       </c>
       <c r="C30"/>
       <c r="D30" s="361" t="s">
-        <v>1026</v>
+        <v>1024</v>
       </c>
       <c r="E30" s="362" t="s">
-        <v>1027</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1025</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31"/>
       <c r="B31"/>
       <c r="C31"/>
       <c r="D31"/>
       <c r="E31"/>
     </row>
-    <row r="32" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="162" t="s">
-        <v>926</v>
+        <v>924</v>
       </c>
       <c r="C32"/>
       <c r="D32" s="361" t="s">
-        <v>1028</v>
+        <v>1026</v>
       </c>
       <c r="E32" s="362" t="s">
-        <v>1029</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1027</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33"/>
       <c r="B33"/>
       <c r="C33"/>
       <c r="D33"/>
       <c r="E33" s="362" t="s">
-        <v>1030</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1028</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34"/>
       <c r="B34"/>
       <c r="C34"/>
       <c r="D34"/>
       <c r="E34"/>
     </row>
-    <row r="35" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="162" t="s">
-        <v>1031</v>
+        <v>1029</v>
       </c>
       <c r="C35"/>
       <c r="D35" s="361" t="s">
+        <v>1031</v>
+      </c>
+      <c r="E35" s="362" t="s">
+        <v>1032</v>
+      </c>
+      <c r="F35" s="422" t="s">
+        <v>1034</v>
+      </c>
+      <c r="G35" s="363" t="s">
         <v>1033</v>
       </c>
-      <c r="E35" s="362" t="s">
-        <v>1034</v>
-      </c>
-      <c r="F35" s="422" t="s">
-        <v>1036</v>
-      </c>
-      <c r="G35" s="363" t="s">
-        <v>1035</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36"/>
       <c r="B36"/>
       <c r="C36"/>
       <c r="D36"/>
       <c r="E36"/>
     </row>
-    <row r="37" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="162" t="s">
-        <v>1032</v>
+        <v>1030</v>
       </c>
       <c r="C37"/>
       <c r="D37" s="361" t="s">
+        <v>1035</v>
+      </c>
+      <c r="E37" s="362" t="s">
+        <v>1036</v>
+      </c>
+      <c r="F37" s="422" t="s">
         <v>1037</v>
       </c>
-      <c r="E37" s="362" t="s">
+      <c r="G37" s="363" t="s">
         <v>1038</v>
       </c>
-      <c r="F37" s="422" t="s">
-        <v>1039</v>
-      </c>
-      <c r="G37" s="363" t="s">
-        <v>1040</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38"/>
       <c r="B38"/>
       <c r="C38"/>
       <c r="D38"/>
       <c r="E38"/>
     </row>
-    <row r="39" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="162" t="s">
         <v>729</v>
       </c>
@@ -24342,21 +24342,21 @@
         <v>723</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40"/>
       <c r="D40" s="361" t="s">
         <v>731</v>
       </c>
       <c r="E40"/>
     </row>
-    <row r="41" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41"/>
       <c r="B41"/>
       <c r="C41"/>
       <c r="D41"/>
       <c r="E41"/>
     </row>
-    <row r="42" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="162" t="s">
         <v>263</v>
       </c>
@@ -24367,19 +24367,19 @@
         <v>723</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43"/>
       <c r="D43"/>
       <c r="E43"/>
     </row>
-    <row r="44" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44"/>
       <c r="B44"/>
       <c r="C44"/>
       <c r="D44"/>
       <c r="E44"/>
     </row>
-    <row r="45" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="162" t="s">
         <v>725</v>
       </c>
@@ -24390,11 +24390,11 @@
         <v>723</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46"/>
       <c r="D46"/>
     </row>
-    <row r="47" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="162" t="s">
         <v>727</v>
       </c>
@@ -24405,20 +24405,20 @@
         <v>723</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48"/>
       <c r="D48"/>
     </row>
-    <row r="49" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49"/>
     </row>
-    <row r="50" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50"/>
     </row>
-    <row r="51" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51"/>
     </row>
-    <row r="52" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52"/>
     </row>
   </sheetData>
@@ -24428,6 +24428,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D428FA97A73D304E91AA59E09D526869" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5184d92e947fddf07e6b6109215ca8be">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8022916f55ab85163ee9a5069dec31d5">
     <xsd:element name="properties">
@@ -24541,12 +24547,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -24557,6 +24557,21 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{53FC0B01-7E98-4633-A4D4-301D890C7458}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2B2DE8A8-9F7C-444A-A54C-B908DB2D8D0F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -24572,21 +24587,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{53FC0B01-7E98-4633-A4D4-301D890C7458}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C69AF5A-C63E-4E3E-821D-D66D815E3725}">
   <ds:schemaRefs>

</xml_diff>